<commit_message>
finish exercise 1.29 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="12090"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -345,10 +345,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -855,7 +855,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -864,10 +864,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -876,7 +876,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1392,10 +1392,10 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -1409,7 +1409,7 @@
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15.5" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:20">
+    <row r="2" customFormat="1" ht="15.5" spans="1:20">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1511,7 +1511,9 @@
       <c r="M2" s="12">
         <v>45514</v>
       </c>
-      <c r="N2" s="16"/>
+      <c r="N2" s="16">
+        <v>45527</v>
+      </c>
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
@@ -1519,7 +1521,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" ht="15.75" spans="1:20">
+    <row r="3" ht="15.5" spans="1:20">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1573,7 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="9" ht="15.75" spans="1:9">
+    <row r="9" ht="15.5" spans="1:9">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -1582,7 +1584,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" ht="15.75" spans="1:9">
+    <row r="10" ht="15.5" spans="1:9">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -1593,7 +1595,7 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" ht="18.75" spans="2:13">
+    <row r="11" ht="17.5" spans="2:13">
       <c r="B11" s="23" t="s">
         <v>36</v>
       </c>
@@ -1609,7 +1611,7 @@
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
     </row>
-    <row r="12" ht="18.75" spans="2:13">
+    <row r="12" ht="17.5" spans="2:13">
       <c r="B12" s="23"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1623,7 +1625,7 @@
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
     </row>
-    <row r="13" ht="18.75" spans="2:12">
+    <row r="13" ht="17.5" spans="2:12">
       <c r="B13" s="23"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1635,7 +1637,7 @@
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
     </row>
-    <row r="14" ht="18.75" spans="2:13">
+    <row r="14" ht="17.5" spans="2:13">
       <c r="B14" s="23"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1648,7 +1650,7 @@
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" ht="18.75" spans="2:13">
+    <row r="15" ht="17.5" spans="2:13">
       <c r="B15" s="23"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1681,7 +1683,7 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -1696,7 +1698,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.5" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15.5" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -1826,7 +1828,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15.5" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>38</v>
       </c>
@@ -1980,7 +1982,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -2129,7 +2131,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2191,7 +2193,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15.5" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2233,7 +2235,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2275,7 +2277,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15.5" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2299,7 +2301,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15.5" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15.5" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2385,7 +2387,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15.5" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -2441,7 +2443,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15.5" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15.5" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -2565,7 +2567,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15.5" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2597,7 +2599,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15.5" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15.5" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2691,7 +2693,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15.5" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -2753,7 +2755,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15.5" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2795,7 +2797,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15.5" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2827,7 +2829,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15.5" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
@@ -2889,7 +2891,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15.5" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2931,7 +2933,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2969,7 +2971,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15.5" spans="1:20">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2991,7 +2993,7 @@
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3013,7 +3015,7 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:20">
+    <row r="29" customFormat="1" ht="15.5" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3035,7 +3037,7 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15.5" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3057,7 +3059,7 @@
       <c r="S30" s="21"/>
       <c r="T30" s="21"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3079,7 +3081,7 @@
       <c r="S31" s="21"/>
       <c r="T31" s="21"/>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15.5" spans="1:20">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3101,7 +3103,7 @@
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15.5" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3123,7 +3125,7 @@
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15.5" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3145,7 +3147,7 @@
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15.5" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3167,7 +3169,7 @@
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15.5" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>

</xml_diff>

<commit_message>
finish exercise 2.4 and 2.5 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="117">
   <si>
     <t>年级</t>
   </si>
@@ -77,84 +77,117 @@
     <t>第10课</t>
   </si>
   <si>
+    <t>初三</t>
+  </si>
+  <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <t>一尔优教育</t>
+  </si>
+  <si>
+    <t>240/2h</t>
+  </si>
+  <si>
+    <t>周六12：00-14：00</t>
+  </si>
+  <si>
+    <t>张佳宁</t>
+  </si>
+  <si>
+    <t>耳鼻喉科专科医院旁巷子201室</t>
+  </si>
+  <si>
+    <t>一中</t>
+  </si>
+  <si>
+    <t>85/100</t>
+  </si>
+  <si>
+    <t>豌豆文化</t>
+  </si>
+  <si>
+    <t>周六17：10-19：10</t>
+  </si>
+  <si>
+    <t>孙朝(zhao)阳</t>
+  </si>
+  <si>
+    <t>天章大厦</t>
+  </si>
+  <si>
+    <t>兵一</t>
+  </si>
+  <si>
+    <t>60/100</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>掌学教育</t>
+  </si>
+  <si>
+    <t>220/2h</t>
+  </si>
+  <si>
+    <t>周日17：00-19：00</t>
+  </si>
+  <si>
+    <t>孙翊原</t>
+  </si>
+  <si>
+    <t>卫生巷88号 6-1-403</t>
+  </si>
+  <si>
+    <t>70/100</t>
+  </si>
+  <si>
+    <t>初一</t>
+  </si>
+  <si>
+    <t>周日19：30-21：30</t>
+  </si>
+  <si>
+    <t>朱思臣</t>
+  </si>
+  <si>
+    <t>新民路29号 3-201</t>
+  </si>
+  <si>
+    <t>98/100</t>
+  </si>
+  <si>
+    <t>转账时间(绿色表示课时费已发)：一尔优当月1号和15号；豌豆文化下月10号；
+博瑞佰艺下月10号；掌学教育和精锐教育都是下月15号
+下次考试目标：孙朝阳：70，张佳宁：95</t>
+  </si>
+  <si>
+    <t>第11课</t>
+  </si>
+  <si>
+    <t>新耀科技</t>
+  </si>
+  <si>
+    <t>180/1.5h</t>
+  </si>
+  <si>
+    <t>周六19：00-20：30</t>
+  </si>
+  <si>
+    <t>宁芮一</t>
+  </si>
+  <si>
+    <t>光明路北小区14-2-503</t>
+  </si>
+  <si>
+    <t>90/150</t>
+  </si>
+  <si>
     <t>初二</t>
-  </si>
-  <si>
-    <t>物理</t>
-  </si>
-  <si>
-    <t>一尔优教育</t>
-  </si>
-  <si>
-    <t>240/2h</t>
-  </si>
-  <si>
-    <t>周六12：00-14：00</t>
-  </si>
-  <si>
-    <t>张佳宁</t>
-  </si>
-  <si>
-    <t>耳鼻喉科专科医院旁巷子201室</t>
-  </si>
-  <si>
-    <t>一中</t>
-  </si>
-  <si>
-    <t>85/100</t>
-  </si>
-  <si>
-    <t>豌豆文化</t>
-  </si>
-  <si>
-    <t>周六17：10-19：10</t>
-  </si>
-  <si>
-    <t>孙朝(zhao)阳</t>
-  </si>
-  <si>
-    <t>天章大厦</t>
-  </si>
-  <si>
-    <t>兵一</t>
-  </si>
-  <si>
-    <t>60/100</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>转账时间(绿色表示课时费已发)：一尔优每月1号和15号；
-豌豆文化每月10号；博瑞佰艺每月10号；
-下次考试目标：孙朝阳：70，张佳宁：95</t>
-  </si>
-  <si>
-    <t>第11课</t>
-  </si>
-  <si>
-    <t>初三</t>
-  </si>
-  <si>
-    <t>数学</t>
-  </si>
-  <si>
-    <t>新耀科技</t>
-  </si>
-  <si>
-    <t>180/1.5h</t>
-  </si>
-  <si>
-    <t>周六19：00-20：30</t>
-  </si>
-  <si>
-    <t>宁芮一</t>
-  </si>
-  <si>
-    <t>光明路北小区14-2-503</t>
-  </si>
-  <si>
-    <t>90/150</t>
   </si>
   <si>
     <t>260/2h</t>
@@ -345,10 +378,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -864,21 +897,21 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1000,7 +1033,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1061,11 +1094,20 @@
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1389,10 +1431,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1400,7 +1442,7 @@
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="7.41666666666667" customWidth="1"/>
-    <col min="5" max="5" width="22.625" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12.375" customWidth="1"/>
     <col min="7" max="7" width="28.25" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
@@ -1573,46 +1615,108 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="9" ht="15.75" spans="1:9">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+    <row r="4" ht="15.75" spans="1:20">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="25">
+        <v>45543</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+    </row>
+    <row r="5" ht="15.75" spans="1:10">
+      <c r="A5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="25">
+        <v>45543</v>
+      </c>
     </row>
     <row r="10" ht="15.75" spans="1:9">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" ht="18.75" spans="2:13">
-      <c r="B11" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+    </row>
+    <row r="11" ht="15.75" spans="1:9">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" ht="18.75" spans="2:13">
-      <c r="B12" s="23"/>
+      <c r="B12" s="24" t="s">
+        <v>48</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1620,13 +1724,13 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-    </row>
-    <row r="13" ht="18.75" spans="2:12">
-      <c r="B13" s="23"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" ht="18.75" spans="2:13">
+      <c r="B13" s="24"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1634,39 +1738,53 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-    </row>
-    <row r="14" ht="18.75" spans="2:13">
-      <c r="B14" s="23"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" ht="18.75" spans="2:12">
+      <c r="B14" s="24"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
+      <c r="I14" s="8"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
     </row>
     <row r="15" ht="18.75" spans="2:13">
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" ht="18.75" spans="2:13">
+      <c r="B16" s="24"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B11:H15"/>
+    <mergeCell ref="B12:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1760,36 +1878,36 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J2" s="9">
         <v>45185</v>
@@ -1830,31 +1948,31 @@
     </row>
     <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>35</v>
@@ -1889,31 +2007,31 @@
     </row>
     <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -1924,31 +2042,31 @@
     </row>
     <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>35</v>
@@ -1984,28 +2102,28 @@
     </row>
     <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>34</v>
@@ -2046,31 +2164,31 @@
     </row>
     <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>35</v>
@@ -2092,31 +2210,31 @@
     </row>
     <row r="8" customFormat="1" ht="17" customHeight="1" spans="1:20">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2133,7 +2251,7 @@
     </row>
     <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -2142,22 +2260,22 @@
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2303,10 +2421,10 @@
     </row>
     <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>22</v>
@@ -2315,19 +2433,19 @@
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>35</v>
@@ -2389,10 +2507,10 @@
     </row>
     <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>22</v>
@@ -2401,19 +2519,19 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>35</v>
@@ -2445,7 +2563,7 @@
     </row>
     <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>21</v>
@@ -2457,19 +2575,19 @@
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>35</v>
@@ -2507,10 +2625,10 @@
     </row>
     <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -2519,19 +2637,19 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>35</v>
@@ -2601,10 +2719,10 @@
     </row>
     <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -2613,19 +2731,19 @@
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>35</v>
@@ -2695,10 +2813,10 @@
     </row>
     <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>29</v>
@@ -2707,19 +2825,19 @@
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>35</v>
@@ -2831,31 +2949,31 @@
     </row>
     <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>35</v>
@@ -3193,7 +3311,7 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="8" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>

</xml_diff>

<commit_message>
finish exercise 2.17 of sicp and update tutor records
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
   <si>
     <t>年级</t>
   </si>
@@ -98,7 +98,7 @@
     <t>耳鼻喉科专科医院旁巷子201室</t>
   </si>
   <si>
-    <t>一中</t>
+    <t>13中</t>
   </si>
   <si>
     <t>85/100</t>
@@ -125,28 +125,97 @@
     <t>/</t>
   </si>
   <si>
+    <t>高一</t>
+  </si>
+  <si>
     <t>数学</t>
   </si>
   <si>
+    <t>300/2h</t>
+  </si>
+  <si>
+    <t>周日15：30-17：30</t>
+  </si>
+  <si>
+    <t>吴雨桐</t>
+  </si>
+  <si>
+    <t>丽园路轩和苑C区 3-2-102</t>
+  </si>
+  <si>
+    <t>60/150</t>
+  </si>
+  <si>
+    <t>450/2h</t>
+  </si>
+  <si>
+    <t>周六16：30-18：30</t>
+  </si>
+  <si>
+    <t>魏子骞</t>
+  </si>
+  <si>
+    <t>幸福路48号二建小区 9-2-302</t>
+  </si>
+  <si>
+    <t>70/100</t>
+  </si>
+  <si>
+    <t>星期天培训</t>
+  </si>
+  <si>
+    <t>220/2h</t>
+  </si>
+  <si>
+    <t>周六21：00-23：00</t>
+  </si>
+  <si>
+    <t>李梦媛</t>
+  </si>
+  <si>
+    <t>铁路局16街晟和家园3号楼2203室</t>
+  </si>
+  <si>
+    <t>70中</t>
+  </si>
+  <si>
+    <t>30/100</t>
+  </si>
+  <si>
+    <t>270/2h</t>
+  </si>
+  <si>
+    <t>周日11：00-13：00</t>
+  </si>
+  <si>
+    <t>刘桐语</t>
+  </si>
+  <si>
+    <t>莲湖路196号博香苑小区6-2-1001</t>
+  </si>
+  <si>
+    <t>126中学</t>
+  </si>
+  <si>
+    <t>130/150</t>
+  </si>
+  <si>
+    <t>精锐教育</t>
+  </si>
+  <si>
+    <t>周日17：00-19：00</t>
+  </si>
+  <si>
+    <t>孙翊原</t>
+  </si>
+  <si>
+    <t>卫生巷88号 6-1-403</t>
+  </si>
+  <si>
+    <t>初一</t>
+  </si>
+  <si>
     <t>掌学教育</t>
-  </si>
-  <si>
-    <t>220/2h</t>
-  </si>
-  <si>
-    <t>周日17：00-19：00</t>
-  </si>
-  <si>
-    <t>孙翊原</t>
-  </si>
-  <si>
-    <t>卫生巷88号 6-1-403</t>
-  </si>
-  <si>
-    <t>70/100</t>
-  </si>
-  <si>
-    <t>初一</t>
   </si>
   <si>
     <t>周日19：30-21：30</t>
@@ -244,9 +313,6 @@
     <t>德泽园三区1-1-202</t>
   </si>
   <si>
-    <t>126中学</t>
-  </si>
-  <si>
     <t>周日18：00-20：00</t>
   </si>
   <si>
@@ -293,9 +359,6 @@
   </si>
   <si>
     <t>邮区中心局小区3-4-602</t>
-  </si>
-  <si>
-    <t>13中</t>
   </si>
   <si>
     <t>李冰惠</t>
@@ -1094,19 +1157,17 @@
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1431,10 +1492,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1444,7 +1505,7 @@
     <col min="4" max="4" width="7.41666666666667" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="30.4166666666667" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="10" width="8.41666666666667" customWidth="1"/>
@@ -1591,7 +1652,7 @@
       <c r="I3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K3" s="12">
@@ -1615,15 +1676,15 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" ht="15.5" spans="1:20">
+    <row r="4" customFormat="1" ht="15.5" spans="1:20">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>38</v>
@@ -1637,135 +1698,288 @@
       <c r="G4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="12" t="s">
         <v>35</v>
       </c>
       <c r="K4" s="25">
-        <v>45543</v>
-      </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-    </row>
-    <row r="5" ht="15.5" spans="1:11">
+        <v>45551</v>
+      </c>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+    </row>
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>33</v>
+      <c r="H5" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="12">
+        <v>45460</v>
+      </c>
+      <c r="L5" s="12">
+        <v>45465</v>
+      </c>
+      <c r="M5" s="12">
+        <v>45514</v>
+      </c>
+      <c r="N5" s="12">
+        <v>45527</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+    </row>
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="25">
+        <v>45551</v>
+      </c>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12">
+        <v>45551</v>
+      </c>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+    </row>
+    <row r="8" ht="15.5" spans="1:20">
+      <c r="A8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="12">
+        <v>45551</v>
+      </c>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+    </row>
+    <row r="9" ht="15.5" spans="1:20">
+      <c r="A9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="26">
         <v>45543</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K9" s="25">
         <v>45550</v>
       </c>
-    </row>
-    <row r="10" ht="15.5" spans="1:9">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" ht="15.5" spans="1:9">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" ht="17.5" spans="2:13">
-      <c r="B12" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-    </row>
-    <row r="13" ht="17.5" spans="2:13">
-      <c r="B13" s="24"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-    </row>
-    <row r="14" ht="17.5" spans="2:12">
-      <c r="B14" s="24"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+    </row>
+    <row r="10" s="22" customFormat="1" ht="15.5"/>
+    <row r="11" s="22" customFormat="1" ht="15.5"/>
+    <row r="12" s="22" customFormat="1" ht="15.5"/>
+    <row r="13" s="22" customFormat="1" ht="15.5" spans="1:9">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+    </row>
+    <row r="14" s="22" customFormat="1" ht="15.5" spans="1:9">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" ht="17.5" spans="2:13">
-      <c r="B15" s="24"/>
+      <c r="B15" s="24" t="s">
+        <v>71</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -1785,9 +1999,48 @@
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
     </row>
+    <row r="17" ht="17.5" spans="2:12">
+      <c r="B17" s="24"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" ht="17.5" spans="2:13">
+      <c r="B18" s="24"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" ht="17.5" spans="2:13">
+      <c r="B19" s="24"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B12:H16"/>
+    <mergeCell ref="B15:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -1881,7 +2134,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="15.5" spans="1:21">
@@ -1889,28 +2142,28 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="J2" s="9">
         <v>45185</v>
@@ -1951,31 +2204,31 @@
     </row>
     <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>35</v>
@@ -2013,28 +2266,28 @@
         <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -2048,28 +2301,28 @@
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>35</v>
@@ -2105,28 +2358,28 @@
     </row>
     <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>34</v>
@@ -2170,28 +2423,28 @@
         <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>35</v>
@@ -2216,28 +2469,28 @@
         <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2263,22 +2516,22 @@
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2427,7 +2680,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>22</v>
@@ -2436,19 +2689,19 @@
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>35</v>
@@ -2513,7 +2766,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>22</v>
@@ -2522,19 +2775,19 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>35</v>
@@ -2578,19 +2831,19 @@
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>35</v>
@@ -2631,7 +2884,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -2640,19 +2893,19 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>35</v>
@@ -2725,7 +2978,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>29</v>
@@ -2734,19 +2987,19 @@
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>35</v>
@@ -2819,7 +3072,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>29</v>
@@ -2828,19 +3081,19 @@
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>35</v>
@@ -2955,28 +3208,28 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>35</v>
@@ -3314,7 +3567,7 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="8" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>

</xml_diff>

<commit_message>
finish exercise 2.21 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="144">
   <si>
     <t>年级</t>
   </si>
@@ -131,13 +131,13 @@
     <t>周六15：30-17：30</t>
   </si>
   <si>
-    <t>唐总儿子</t>
-  </si>
-  <si>
-    <t>马料地街</t>
-  </si>
-  <si>
-    <t>80/100</t>
+    <t>唐润宁</t>
+  </si>
+  <si>
+    <t>西山东街261号 华美·博奥小区 7-3-401</t>
+  </si>
+  <si>
+    <t>13中分校</t>
   </si>
   <si>
     <t>450/2h</t>
@@ -194,7 +194,7 @@
     <t>周日14：00-16：00</t>
   </si>
   <si>
-    <t>刘桐语同学</t>
+    <t>贾梦垚</t>
   </si>
   <si>
     <t>莲湖路196号博香苑小区6-2-1001</t>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>12中</t>
+  </si>
+  <si>
+    <t>80/100</t>
   </si>
   <si>
     <t>优师帮</t>
@@ -456,10 +459,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -966,7 +969,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -975,10 +978,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -987,7 +990,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1504,24 +1507,24 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="7.41666666666667" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="31.125" customWidth="1"/>
+    <col min="7" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="10" width="8.41666666666667" customWidth="1"/>
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15.5" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:20">
+    <row r="2" customFormat="1" ht="15.5" spans="1:20">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1636,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" ht="15.75" spans="1:20">
+    <row r="3" ht="15.5" spans="1:20">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1685,7 +1688,7 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:20">
+    <row r="4" customFormat="1" ht="15.5" spans="1:20">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1707,9 +1710,11 @@
       <c r="G4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>35</v>
@@ -1725,7 +1730,7 @@
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1775,7 +1780,7 @@
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1809,7 +1814,9 @@
       <c r="K6" s="20">
         <v>45551</v>
       </c>
-      <c r="L6" s="22"/>
+      <c r="L6" s="20">
+        <v>45556</v>
+      </c>
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
@@ -1819,7 +1826,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1863,7 +1870,7 @@
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
     </row>
-    <row r="8" customFormat="1" ht="15.75" spans="1:20">
+    <row r="8" customFormat="1" ht="15.5" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1905,7 +1912,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
     </row>
-    <row r="9" ht="15.75" spans="1:20">
+    <row r="9" ht="15.5" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1937,7 +1944,7 @@
         <v>35</v>
       </c>
       <c r="K9" s="12">
-        <v>45551</v>
+        <v>45543</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -1949,7 +1956,7 @@
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" ht="15.75" spans="1:20">
+    <row r="10" ht="15.5" spans="1:20">
       <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
@@ -1993,7 +2000,7 @@
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
@@ -2037,10 +2044,10 @@
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
     </row>
-    <row r="12" s="22" customFormat="1" ht="15.75"/>
-    <row r="13" s="22" customFormat="1" ht="15.75"/>
-    <row r="14" s="22" customFormat="1" ht="15.75"/>
-    <row r="15" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="12" s="22" customFormat="1" ht="15.5"/>
+    <row r="13" s="22" customFormat="1" ht="15.5"/>
+    <row r="14" s="22" customFormat="1" ht="15.5"/>
+    <row r="15" s="22" customFormat="1" ht="15.5" spans="1:9">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -2051,7 +2058,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="16" s="22" customFormat="1" ht="15.5" spans="1:9">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2062,7 +2069,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" ht="18.75" spans="2:13">
+    <row r="17" ht="17.5" spans="2:13">
       <c r="B17" s="24" t="s">
         <v>78</v>
       </c>
@@ -2078,7 +2085,7 @@
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
     </row>
-    <row r="18" ht="18.75" spans="2:13">
+    <row r="18" ht="17.5" spans="2:13">
       <c r="B18" s="24"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2092,7 +2099,7 @@
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
     </row>
-    <row r="19" ht="18.75" spans="2:12">
+    <row r="19" ht="17.5" spans="2:12">
       <c r="B19" s="24"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2104,7 +2111,7 @@
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
     </row>
-    <row r="20" ht="18.75" spans="2:13">
+    <row r="20" ht="17.5" spans="2:13">
       <c r="B20" s="24"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2117,7 +2124,7 @@
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" ht="18.75" spans="2:13">
+    <row r="21" ht="17.5" spans="2:13">
       <c r="B21" s="24"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2150,7 +2157,7 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2165,7 +2172,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.5" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15.5" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2295,7 +2302,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>86</v>
       </c>
@@ -2321,7 +2328,7 @@
         <v>90</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>35</v>
@@ -2354,7 +2361,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15.5" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2362,25 +2369,25 @@
         <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -2389,7 +2396,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2397,10 +2404,10 @@
         <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>82</v>
@@ -2449,7 +2456,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -2457,19 +2464,19 @@
         <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>56</v>
@@ -2511,7 +2518,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2525,19 +2532,19 @@
         <v>87</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>35</v>
@@ -2565,25 +2572,25 @@
         <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2598,7 +2605,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2609,22 +2616,22 @@
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2660,7 +2667,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15.5" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2702,7 +2709,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2744,7 +2751,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15.5" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2768,7 +2775,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15.5" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2782,13 +2789,13 @@
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>27</v>
@@ -2830,7 +2837,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15.5" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2854,7 +2861,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15.5" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2868,19 +2875,19 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>35</v>
@@ -2910,7 +2917,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15.5" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2924,19 +2931,19 @@
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>35</v>
@@ -2972,7 +2979,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15.5" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2986,19 +2993,19 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>35</v>
@@ -3034,7 +3041,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15.5" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3066,7 +3073,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15.5" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3080,19 +3087,19 @@
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>35</v>
@@ -3128,7 +3135,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15.5" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3160,7 +3167,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15.5" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3174,19 +3181,19 @@
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>35</v>
@@ -3222,7 +3229,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15.5" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3264,7 +3271,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15.5" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3296,7 +3303,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15.5" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3304,25 +3311,25 @@
         <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>35</v>
@@ -3358,7 +3365,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15.5" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3400,7 +3407,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3438,7 +3445,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15.5" spans="1:20">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3460,7 +3467,7 @@
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3482,7 +3489,7 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:20">
+    <row r="29" customFormat="1" ht="15.5" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3504,7 +3511,7 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15.5" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3526,7 +3533,7 @@
       <c r="S30" s="21"/>
       <c r="T30" s="21"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3548,7 +3555,7 @@
       <c r="S31" s="21"/>
       <c r="T31" s="21"/>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15.5" spans="1:20">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3570,7 +3577,7 @@
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15.5" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3592,7 +3599,7 @@
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15.5" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3614,7 +3621,7 @@
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15.5" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3636,7 +3643,7 @@
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15.5" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3660,7 +3667,7 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>

</xml_diff>

<commit_message>
finish reading chapter 1-4 of <Animal Farm>
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -1114,7 +1114,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1181,12 +1181,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1514,7 +1508,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1771,10 +1765,10 @@
       <c r="K5" s="12">
         <v>45552</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="26"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
@@ -1864,10 +1858,10 @@
       <c r="L7" s="9">
         <v>45557</v>
       </c>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
@@ -2086,10 +2080,10 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
     </row>
     <row r="18" ht="17.5" spans="2:13">
       <c r="B18" s="24"/>
@@ -2100,10 +2094,10 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
     </row>
     <row r="19" ht="17.5" spans="2:12">
       <c r="B19" s="24"/>
@@ -2114,8 +2108,8 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" ht="17.5" spans="2:13">
       <c r="B20" s="24"/>
@@ -2125,10 +2119,10 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
     </row>
     <row r="21" ht="17.5" spans="2:13">
       <c r="B21" s="24"/>
@@ -2139,10 +2133,10 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finish exercise 2.34 and 2.35 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -459,10 +459,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -969,7 +969,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -978,10 +978,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -990,7 +990,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1509,10 +1509,10 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -1526,7 +1526,7 @@
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15.5" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:20">
+    <row r="2" customFormat="1" ht="15.5" spans="1:20">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" ht="15.75" spans="1:20">
+    <row r="3" ht="15.5" spans="1:20">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="S3" s="16"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:20">
+    <row r="4" customFormat="1" ht="15.5" spans="1:20">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1813,7 +1813,9 @@
       <c r="L6" s="20">
         <v>45556</v>
       </c>
-      <c r="M6" s="22"/>
+      <c r="M6" s="20">
+        <v>45563</v>
+      </c>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
@@ -1822,7 +1824,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1859,7 +1861,9 @@
       <c r="L7" s="9">
         <v>45557</v>
       </c>
-      <c r="M7" s="25"/>
+      <c r="M7" s="9">
+        <v>45563</v>
+      </c>
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
@@ -1868,7 +1872,7 @@
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
     </row>
-    <row r="8" customFormat="1" ht="15.75" spans="1:20">
+    <row r="8" customFormat="1" ht="15.5" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1912,7 +1916,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
     </row>
-    <row r="9" ht="15.75" spans="1:20">
+    <row r="9" ht="15.5" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1956,7 +1960,7 @@
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" ht="15.75" spans="1:20">
+    <row r="10" ht="15.5" spans="1:20">
       <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
@@ -2002,7 +2006,7 @@
       <c r="S10" s="22"/>
       <c r="T10" s="22"/>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="5" t="s">
         <v>72</v>
       </c>
@@ -2046,10 +2050,10 @@
       <c r="S11" s="22"/>
       <c r="T11" s="22"/>
     </row>
-    <row r="12" s="22" customFormat="1" ht="15.75"/>
-    <row r="13" s="22" customFormat="1" ht="15.75"/>
-    <row r="14" s="22" customFormat="1" ht="15.75"/>
-    <row r="15" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="12" s="22" customFormat="1" ht="15.5"/>
+    <row r="13" s="22" customFormat="1" ht="15.5"/>
+    <row r="14" s="22" customFormat="1" ht="15.5"/>
+    <row r="15" s="22" customFormat="1" ht="15.5" spans="1:9">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -2060,7 +2064,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="16" s="22" customFormat="1" ht="15.5" spans="1:9">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2071,7 +2075,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" ht="18.75" spans="2:13">
+    <row r="17" ht="17.5" spans="2:13">
       <c r="B17" s="24" t="s">
         <v>78</v>
       </c>
@@ -2087,7 +2091,7 @@
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
     </row>
-    <row r="18" ht="18.75" spans="2:13">
+    <row r="18" ht="17.5" spans="2:13">
       <c r="B18" s="24"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2101,7 +2105,7 @@
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
     </row>
-    <row r="19" ht="18.75" spans="2:12">
+    <row r="19" ht="17.5" spans="2:12">
       <c r="B19" s="24"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2113,7 +2117,7 @@
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" ht="18.75" spans="2:13">
+    <row r="20" ht="17.5" spans="2:13">
       <c r="B20" s="24"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2126,7 +2130,7 @@
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" ht="18.75" spans="2:13">
+    <row r="21" ht="17.5" spans="2:13">
       <c r="B21" s="24"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2159,7 +2163,7 @@
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2174,7 +2178,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.5" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15.5" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>86</v>
       </c>
@@ -2363,7 +2367,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15.5" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2458,7 +2462,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -2520,7 +2524,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2607,7 +2611,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2669,7 +2673,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15.5" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2711,7 +2715,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2753,7 +2757,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15.5" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2777,7 +2781,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15.5" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2839,7 +2843,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15.5" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2863,7 +2867,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15.5" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2919,7 +2923,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15.5" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15.5" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3043,7 +3047,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15.5" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3075,7 +3079,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15.5" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15.5" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3169,7 +3173,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15.5" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3231,7 +3235,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15.5" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3273,7 +3277,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15.5" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3305,7 +3309,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15.5" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15.5" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3409,7 +3413,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3447,7 +3451,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15.5" spans="1:20">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3469,7 +3473,7 @@
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3491,7 +3495,7 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:20">
+    <row r="29" customFormat="1" ht="15.5" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3513,7 +3517,7 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15.5" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3535,7 +3539,7 @@
       <c r="S30" s="21"/>
       <c r="T30" s="21"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3557,7 +3561,7 @@
       <c r="S31" s="21"/>
       <c r="T31" s="21"/>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15.5" spans="1:20">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3579,7 +3583,7 @@
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15.5" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3601,7 +3605,7 @@
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15.5" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3623,7 +3627,7 @@
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15.5" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3645,7 +3649,7 @@
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15.5" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>

</xml_diff>

<commit_message>
finish exercise 2.41 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -245,8 +245,8 @@
     <t>60/150</t>
   </si>
   <si>
-    <t>转账时间(绿色表示课时费已发)：豌豆文化每月10号；星期天培训下个月20号；
-掌学教育和精锐教育都是下月15号
+    <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
+星期天培训下个月20号；掌学教育和精锐教育都是下月15号
 下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100</t>
   </si>
   <si>
@@ -459,10 +459,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -645,7 +645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,6 +661,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,31 +966,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -996,10 +1002,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1020,28 +1026,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1050,19 +1056,16 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1074,38 +1077,41 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1169,6 +1175,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1496,10 +1505,10 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -1513,7 +1522,7 @@
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:20">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1584,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:20">
+    <row r="2" customFormat="1" ht="15.75" spans="1:20">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1629,7 +1638,7 @@
       <c r="S2" s="16"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:18">
+    <row r="3" customFormat="1" ht="15.75" spans="1:18">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1666,7 +1675,7 @@
       <c r="L3" s="20">
         <v>45566</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="24">
         <v>45574</v>
       </c>
       <c r="N3" s="22"/>
@@ -1675,7 +1684,7 @@
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:18">
+    <row r="4" customFormat="1" ht="15.75" spans="1:18">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1726,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1771,7 +1780,7 @@
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1814,14 +1823,14 @@
       <c r="N6" s="9">
         <v>45567</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1861,15 +1870,15 @@
       <c r="M7" s="9">
         <v>45572</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
     </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+    <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1917,7 +1926,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
@@ -1963,7 +1972,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
     </row>
-    <row r="10" ht="15.5" spans="1:20">
+    <row r="10" ht="15.75" spans="1:20">
       <c r="A10" s="5" t="s">
         <v>69</v>
       </c>
@@ -2007,12 +2016,12 @@
       <c r="S10" s="20"/>
       <c r="T10" s="20"/>
     </row>
-    <row r="11" s="22" customFormat="1" ht="15.5"/>
-    <row r="12" s="22" customFormat="1" ht="15.5"/>
-    <row r="13" s="22" customFormat="1" ht="15.5"/>
-    <row r="14" s="22" customFormat="1" ht="15.5"/>
-    <row r="15" s="22" customFormat="1" ht="15.5"/>
-    <row r="16" s="22" customFormat="1" ht="15.5" spans="1:9">
+    <row r="11" s="22" customFormat="1" ht="15.75"/>
+    <row r="12" s="22" customFormat="1" ht="15.75"/>
+    <row r="13" s="22" customFormat="1" ht="15.75"/>
+    <row r="14" s="22" customFormat="1" ht="15.75"/>
+    <row r="15" s="22" customFormat="1" ht="15.75"/>
+    <row r="16" s="22" customFormat="1" ht="15.75" spans="1:9">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2023,7 +2032,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" s="22" customFormat="1" ht="15.5" spans="1:9">
+    <row r="17" s="22" customFormat="1" ht="15.75" spans="1:9">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -2034,7 +2043,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" ht="17.5" spans="2:13">
+    <row r="18" ht="18.75" spans="2:13">
       <c r="B18" s="8" t="s">
         <v>76</v>
       </c>
@@ -2045,12 +2054,12 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-    </row>
-    <row r="19" ht="17.5" spans="2:13">
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" ht="18.75" spans="2:13">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2059,12 +2068,12 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-    </row>
-    <row r="20" ht="17.5" spans="2:12">
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" ht="18.75" spans="2:12">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2073,10 +2082,10 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-    </row>
-    <row r="21" ht="17.5" spans="2:13">
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" ht="18.75" spans="2:13">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2085,12 +2094,12 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-    </row>
-    <row r="22" ht="17.5" spans="2:13">
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" ht="18.75" spans="2:13">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2099,10 +2108,10 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2123,7 +2132,7 @@
       <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2138,7 +2147,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:21">
+    <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:19">
+    <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>84</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:11">
+    <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2362,7 +2371,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2422,7 +2431,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>84</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2571,7 +2580,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2675,7 +2684,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2717,7 +2726,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.5" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2741,7 +2750,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.5" spans="1:20">
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2803,7 +2812,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.5" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2827,7 +2836,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.5" spans="1:20">
+    <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2883,7 +2892,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.5" spans="1:20">
+    <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2945,7 +2954,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.5" spans="1:20">
+    <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3007,7 +3016,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.5" spans="1:20">
+    <row r="18" customFormat="1" ht="15.75" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3039,7 +3048,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.5" spans="1:20">
+    <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3101,7 +3110,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.5" spans="1:20">
+    <row r="20" customFormat="1" ht="15.75" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3133,7 +3142,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.5" spans="1:20">
+    <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3195,7 +3204,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.5" spans="1:20">
+    <row r="22" customFormat="1" ht="15.75" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3237,7 +3246,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.5" spans="1:20">
+    <row r="23" customFormat="1" ht="15.75" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3269,7 +3278,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.5" spans="1:20">
+    <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3331,7 +3340,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.5" spans="1:20">
+    <row r="25" customFormat="1" ht="15.75" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3373,7 +3382,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3411,7 +3420,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.5" spans="1:20">
+    <row r="27" customFormat="1" ht="15.75" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
@@ -3461,7 +3470,7 @@
       <c r="S27" s="16"/>
       <c r="T27" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15.5" spans="1:20">
+    <row r="29" customFormat="1" ht="15.75" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3483,7 +3492,7 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.5" spans="1:20">
+    <row r="30" customFormat="1" ht="15.75" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3505,7 +3514,7 @@
       <c r="S30" s="21"/>
       <c r="T30" s="21"/>
     </row>
-    <row r="31" customFormat="1" ht="15.5" spans="1:20">
+    <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3527,7 +3536,7 @@
       <c r="S31" s="21"/>
       <c r="T31" s="21"/>
     </row>
-    <row r="32" customFormat="1" ht="15.5" spans="1:20">
+    <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3549,7 +3558,7 @@
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
     </row>
-    <row r="33" customFormat="1" ht="15.5" spans="1:20">
+    <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3571,7 +3580,7 @@
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
     </row>
-    <row r="34" customFormat="1" ht="15.5" spans="1:20">
+    <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3593,7 +3602,7 @@
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
     </row>
-    <row r="35" customFormat="1" ht="15.5" spans="1:20">
+    <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3615,7 +3624,7 @@
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
     </row>
-    <row r="36" customFormat="1" ht="15.5" spans="1:20">
+    <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>

</xml_diff>

<commit_message>
finish exercise 2.48 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -221,29 +221,8 @@
     <t>70/90</t>
   </si>
   <si>
-    <t>高一</t>
-  </si>
-  <si>
-    <t>一尔优教育</t>
-  </si>
-  <si>
-    <t>320/2h</t>
-  </si>
-  <si>
-    <t>周日15：30-17：30</t>
-  </si>
-  <si>
-    <t>吴雨桐</t>
-  </si>
-  <si>
-    <t>丽园路轩和苑C区 3-2-102</t>
-  </si>
-  <si>
-    <t>60/150</t>
-  </si>
-  <si>
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
-星期天培训下个月20号；掌学教育和精锐教育都是下月15号
+精锐教育是当月15号；星期天培训下个月20号；掌学教育是下月15号
 下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100
 李梦媛10月12日只上了半节课</t>
   </si>
@@ -323,6 +302,9 @@
     <t>德泽园三区1-1-202</t>
   </si>
   <si>
+    <t>一尔优教育</t>
+  </si>
+  <si>
     <t>周日18：00-20：00</t>
   </si>
   <si>
@@ -444,6 +426,24 @@
   </si>
   <si>
     <t>85/100</t>
+  </si>
+  <si>
+    <t>高一</t>
+  </si>
+  <si>
+    <t>320/2h</t>
+  </si>
+  <si>
+    <t>周日15：30-17：30</t>
+  </si>
+  <si>
+    <t>吴雨桐</t>
+  </si>
+  <si>
+    <t>丽园路轩和苑C区 3-2-102</t>
+  </si>
+  <si>
+    <t>60/150</t>
   </si>
   <si>
     <t xml:space="preserve">绿色表示课时费已发；
@@ -458,8 +458,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -973,19 +973,19 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1164,13 +1164,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1613,20 +1613,20 @@
       <c r="J2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2" s="21">
         <v>45556</v>
       </c>
-      <c r="L2" s="20">
+      <c r="L2" s="21">
         <v>45566</v>
       </c>
       <c r="M2" s="24">
         <v>45574</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
     </row>
     <row r="3" customFormat="1" ht="15.75" spans="1:20">
       <c r="A3" s="5" t="s">
@@ -1665,16 +1665,16 @@
       <c r="L3" s="9">
         <v>45557</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="21">
         <v>45578</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
     </row>
     <row r="4" customFormat="1" ht="15.75" spans="1:20">
       <c r="A4" s="5" t="s">
@@ -1723,8 +1723,8 @@
         <v>45578</v>
       </c>
       <c r="P4" s="25"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
     </row>
@@ -1770,11 +1770,11 @@
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="5" t="s">
@@ -1807,32 +1807,32 @@
       <c r="J6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="21">
         <v>45551</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="21">
         <v>45556</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="21">
         <v>45563</v>
       </c>
-      <c r="N6" s="20">
+      <c r="N6" s="21">
         <v>45566</v>
       </c>
-      <c r="O6" s="20">
+      <c r="O6" s="21">
         <v>45567</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="21">
         <v>45572</v>
       </c>
-      <c r="Q6" s="20">
+      <c r="Q6" s="21">
         <v>45577</v>
       </c>
-      <c r="R6" s="20">
+      <c r="R6" s="21">
         <v>45578</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
     </row>
     <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
@@ -1868,19 +1868,19 @@
       <c r="K7" s="12">
         <v>45543</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="9">
         <v>45566</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="9">
         <v>45567</v>
       </c>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
     </row>
     <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="5" t="s">
@@ -1928,7 +1928,7 @@
       <c r="O8" s="12">
         <v>45465</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="21">
         <v>45572</v>
       </c>
       <c r="Q8" s="16"/>
@@ -1978,56 +1978,12 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" ht="15.75" spans="1:20">
-      <c r="A10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="20">
-        <v>45551</v>
-      </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-    </row>
-    <row r="11" s="22" customFormat="1" ht="15.75"/>
-    <row r="12" s="22" customFormat="1" ht="15.75"/>
-    <row r="13" s="22" customFormat="1" ht="15.75"/>
-    <row r="14" s="22" customFormat="1" ht="15.75"/>
-    <row r="15" s="22" customFormat="1" ht="15.75"/>
-    <row r="16" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="11" s="20" customFormat="1" ht="15.75"/>
+    <row r="12" s="20" customFormat="1" ht="15.75"/>
+    <row r="13" s="20" customFormat="1" ht="15.75"/>
+    <row r="14" s="20" customFormat="1" ht="15.75"/>
+    <row r="15" s="20" customFormat="1" ht="15.75"/>
+    <row r="16" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2038,7 +1994,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" s="22" customFormat="1" ht="15.75" spans="1:9">
+    <row r="17" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -2051,7 +2007,7 @@
     </row>
     <row r="18" ht="18.75" spans="2:13">
       <c r="B18" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2132,10 +2088,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2215,7 +2171,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="15.75" spans="1:21">
@@ -2226,25 +2182,25 @@
         <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J2" s="9">
         <v>45185</v>
@@ -2285,7 +2241,7 @@
     </row>
     <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>21</v>
@@ -2294,22 +2250,22 @@
         <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>22</v>
@@ -2350,25 +2306,25 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -2385,25 +2341,25 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>22</v>
@@ -2439,25 +2395,25 @@
     </row>
     <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>41</v>
@@ -2507,25 +2463,25 @@
         <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>22</v>
@@ -2553,25 +2509,25 @@
         <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2594,25 +2550,25 @@
         <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2764,25 +2720,25 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>22</v>
@@ -2850,25 +2806,25 @@
         <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>22</v>
@@ -2912,16 +2868,16 @@
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>52</v>
@@ -2974,19 +2930,19 @@
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>22</v>
@@ -3068,16 +3024,16 @@
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>28</v>
@@ -3162,19 +3118,19 @@
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>22</v>
@@ -3292,25 +3248,25 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>22</v>
@@ -3434,25 +3390,25 @@
         <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>66</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J27" s="12">
         <v>45451</v>
@@ -3476,27 +3432,49 @@
       <c r="S27" s="16"/>
       <c r="T27" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:20">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
+    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A28" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="9">
+        <v>45551</v>
+      </c>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
     </row>
     <row r="30" customFormat="1" ht="15.75" spans="1:20">
       <c r="A30" s="4"/>
@@ -3508,17 +3486,17 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
     </row>
     <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="4"/>
@@ -3530,17 +3508,17 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
     </row>
     <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="4"/>
@@ -3552,17 +3530,17 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
     </row>
     <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
@@ -3574,17 +3552,17 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
     </row>
     <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="4"/>
@@ -3596,17 +3574,17 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
     </row>
     <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4"/>
@@ -3618,17 +3596,17 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
     </row>
     <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
@@ -3640,34 +3618,44 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-    </row>
-    <row r="37" spans="2:11">
-      <c r="B37" s="8" t="s">
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+    </row>
+    <row r="37" customFormat="1" ht="15.75" spans="1:20">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-    </row>
-    <row r="38" spans="2:11">
-      <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -3737,6 +3725,18 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="61">
@@ -3800,7 +3800,7 @@
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="J24:J26"/>
-    <mergeCell ref="B37:K43"/>
+    <mergeCell ref="B38:K44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
finish exercise 2.56 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -457,9 +457,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -964,21 +964,21 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1109,7 +1109,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1175,9 +1175,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1671,7 +1668,7 @@
       <c r="L3" s="9">
         <v>45557</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="9">
         <v>45578</v>
       </c>
       <c r="N3" s="21">
@@ -1733,8 +1730,8 @@
       <c r="P4" s="9">
         <v>45585</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
     </row>
@@ -1750,15 +1747,15 @@
       <c r="I5" s="4"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
     </row>
     <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="5" t="s">
@@ -1803,7 +1800,7 @@
       <c r="N6" s="9">
         <v>45585</v>
       </c>
-      <c r="O6" s="26"/>
+      <c r="O6" s="25"/>
       <c r="P6" s="20"/>
       <c r="R6" s="20"/>
       <c r="S6" s="20"/>
@@ -2053,10 +2050,10 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
     </row>
     <row r="20" ht="18.75" spans="2:13">
       <c r="B20" s="8"/>
@@ -2067,10 +2064,10 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
     </row>
     <row r="21" ht="18.75" spans="2:12">
       <c r="B21" s="8"/>
@@ -2081,8 +2078,8 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" ht="18.75" spans="2:13">
       <c r="B22" s="8"/>
@@ -2093,10 +2090,10 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
     </row>
     <row r="23" ht="18.75" spans="2:13">
       <c r="B23" s="8"/>
@@ -2107,10 +2104,10 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
finish exercise 2.67 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12330"/>
+    <workbookView windowWidth="25200" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="143">
   <si>
     <t>年级</t>
   </si>
@@ -457,10 +457,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -964,7 +964,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -973,10 +973,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -985,7 +985,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1504,10 +1504,10 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -1516,12 +1516,11 @@
     <col min="6" max="6" width="12.375" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="9" width="9.125" customWidth="1"/>
-    <col min="10" max="10" width="8.41666666666667" customWidth="1"/>
+    <col min="9" max="10" width="9.125" customWidth="1"/>
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:20">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1583,7 +1582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:18">
+    <row r="2" customFormat="1" ht="15.75" spans="1:18">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1611,29 +1610,26 @@
       <c r="I2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>22</v>
+      <c r="J2" s="21">
+        <v>45556</v>
       </c>
       <c r="K2" s="21">
-        <v>45556</v>
-      </c>
-      <c r="L2" s="21">
         <v>45566</v>
       </c>
-      <c r="M2" s="24">
+      <c r="L2" s="24">
         <v>45574</v>
       </c>
+      <c r="M2" s="21">
+        <v>45584</v>
+      </c>
       <c r="N2" s="21">
-        <v>45584</v>
-      </c>
-      <c r="O2" s="21">
         <v>45591</v>
       </c>
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:20">
+    <row r="3" customFormat="1" ht="15.75" spans="1:20">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1685,7 +1681,7 @@
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:20">
+    <row r="4" customFormat="1" ht="15.75" spans="1:20">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1741,7 +1737,7 @@
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1763,7 +1759,7 @@
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1814,7 +1810,7 @@
       <c r="S6" s="20"/>
       <c r="T6" s="20"/>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -1876,7 +1872,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+    <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1916,10 +1912,10 @@
       <c r="M8" s="9">
         <v>45567</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="9">
         <v>45585</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="9">
         <v>45592</v>
       </c>
       <c r="P8" s="21"/>
@@ -1928,7 +1924,7 @@
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1982,7 +1978,7 @@
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:18">
+    <row r="10" customFormat="1" ht="15.75" spans="1:18">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -2024,12 +2020,12 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="12" s="20" customFormat="1" ht="15.5"/>
-    <row r="13" s="20" customFormat="1" ht="15.5"/>
-    <row r="14" s="20" customFormat="1" ht="15.5"/>
-    <row r="15" s="20" customFormat="1" ht="15.5"/>
-    <row r="16" s="20" customFormat="1" ht="15.5"/>
-    <row r="17" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="12" s="20" customFormat="1" ht="15.75"/>
+    <row r="13" s="20" customFormat="1" ht="15.75"/>
+    <row r="14" s="20" customFormat="1" ht="15.75"/>
+    <row r="15" s="20" customFormat="1" ht="15.75"/>
+    <row r="16" s="20" customFormat="1" ht="15.75"/>
+    <row r="17" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -2040,7 +2036,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="18" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -2051,7 +2047,7 @@
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
     </row>
-    <row r="19" ht="17.5" spans="2:13">
+    <row r="19" ht="18.75" spans="2:13">
       <c r="B19" s="8" t="s">
         <v>68</v>
       </c>
@@ -2067,7 +2063,7 @@
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
     </row>
-    <row r="20" ht="17.5" spans="2:13">
+    <row r="20" ht="18.75" spans="2:13">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2081,7 +2077,7 @@
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" ht="17.5" spans="2:12">
+    <row r="21" ht="18.75" spans="2:12">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2093,7 +2089,7 @@
       <c r="K21" s="25"/>
       <c r="L21" s="25"/>
     </row>
-    <row r="22" ht="17.5" spans="2:13">
+    <row r="22" ht="18.75" spans="2:13">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2107,7 +2103,7 @@
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
     </row>
-    <row r="23" ht="17.5" spans="2:13">
+    <row r="23" ht="18.75" spans="2:13">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2150,7 +2146,7 @@
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2165,7 +2161,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2226,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:21">
+    <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2295,7 +2291,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:19">
+    <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
@@ -2354,7 +2350,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:11">
+    <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2389,7 +2385,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2449,7 +2445,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>76</v>
       </c>
@@ -2511,7 +2507,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2598,7 +2594,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2660,7 +2656,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2702,7 +2698,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2744,7 +2740,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.5" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2768,7 +2764,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.5" spans="1:20">
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2830,7 +2826,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.5" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2854,7 +2850,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.5" spans="1:20">
+    <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2910,7 +2906,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.5" spans="1:20">
+    <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -2972,7 +2968,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.5" spans="1:20">
+    <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3034,7 +3030,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.5" spans="1:20">
+    <row r="18" customFormat="1" ht="15.75" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3066,7 +3062,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.5" spans="1:20">
+    <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3124,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.5" spans="1:20">
+    <row r="20" customFormat="1" ht="15.75" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3160,7 +3156,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.5" spans="1:20">
+    <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3222,7 +3218,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.5" spans="1:20">
+    <row r="22" customFormat="1" ht="15.75" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3264,7 +3260,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.5" spans="1:20">
+    <row r="23" customFormat="1" ht="15.75" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3296,7 +3292,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.5" spans="1:20">
+    <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3358,7 +3354,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.5" spans="1:20">
+    <row r="25" customFormat="1" ht="15.75" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3400,7 +3396,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3438,7 +3434,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.5" spans="1:20">
+    <row r="27" customFormat="1" ht="15.75" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
@@ -3488,7 +3484,7 @@
       <c r="S27" s="16"/>
       <c r="T27" s="16"/>
     </row>
-    <row r="28" customFormat="1" ht="15.5" spans="1:20">
+    <row r="28" customFormat="1" ht="15.75" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>136</v>
       </c>
@@ -3532,7 +3528,7 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.5" spans="1:20">
+    <row r="30" customFormat="1" ht="15.75" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3554,7 +3550,7 @@
       <c r="S30" s="22"/>
       <c r="T30" s="22"/>
     </row>
-    <row r="31" customFormat="1" ht="15.5" spans="1:20">
+    <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3576,7 +3572,7 @@
       <c r="S31" s="22"/>
       <c r="T31" s="22"/>
     </row>
-    <row r="32" customFormat="1" ht="15.5" spans="1:20">
+    <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3598,7 +3594,7 @@
       <c r="S32" s="22"/>
       <c r="T32" s="22"/>
     </row>
-    <row r="33" customFormat="1" ht="15.5" spans="1:20">
+    <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3620,7 +3616,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.5" spans="1:20">
+    <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3642,7 +3638,7 @@
       <c r="S34" s="22"/>
       <c r="T34" s="22"/>
     </row>
-    <row r="35" customFormat="1" ht="15.5" spans="1:20">
+    <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3664,7 +3660,7 @@
       <c r="S35" s="22"/>
       <c r="T35" s="22"/>
     </row>
-    <row r="36" customFormat="1" ht="15.5" spans="1:20">
+    <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3686,7 +3682,7 @@
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
     </row>
-    <row r="37" customFormat="1" ht="15.5" spans="1:20">
+    <row r="37" customFormat="1" ht="15.75" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>

</xml_diff>

<commit_message>
finish exercise 2.68-2.70 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -643,7 +643,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,12 +659,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,10 +961,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -979,16 +973,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1000,52 +994,52 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1054,16 +1048,19 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1075,41 +1072,38 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1173,12 +1167,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1506,7 +1494,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1612,22 +1600,22 @@
       <c r="I2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2" s="9">
         <v>45556</v>
       </c>
-      <c r="K2" s="21">
+      <c r="K2" s="9">
         <v>45566</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="9">
         <v>45574</v>
       </c>
-      <c r="M2" s="21">
+      <c r="M2" s="9">
         <v>45584</v>
       </c>
-      <c r="N2" s="21">
+      <c r="N2" s="9">
         <v>45591</v>
       </c>
-      <c r="O2" s="21">
+      <c r="O2" s="9">
         <v>45598</v>
       </c>
       <c r="P2" s="20"/>
@@ -1674,10 +1662,10 @@
       <c r="M3" s="9">
         <v>45578</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="9">
         <v>45584</v>
       </c>
-      <c r="O3" s="21">
+      <c r="O3" s="9">
         <v>45591</v>
       </c>
       <c r="P3" s="21">
@@ -1763,8 +1751,8 @@
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
     </row>
@@ -1897,10 +1885,10 @@
       <c r="K8" s="21">
         <v>45599</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
@@ -2095,10 +2083,10 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" ht="17.5" spans="2:13">
       <c r="B21" s="8"/>
@@ -2109,10 +2097,10 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" ht="17.5" spans="2:12">
       <c r="B22" s="8"/>
@@ -2123,8 +2111,8 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
     </row>
     <row r="23" ht="17.5" spans="2:13">
       <c r="B23" s="8"/>
@@ -2135,10 +2123,10 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" ht="17.5" spans="2:13">
       <c r="B24" s="8"/>
@@ -2149,10 +2137,10 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="21">

</xml_diff>

<commit_message>
finish exercise 2.71-2.72 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -1494,7 +1494,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1995,7 +1995,7 @@
       <c r="O10" s="12">
         <v>45465</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="9">
         <v>45572</v>
       </c>
       <c r="Q10" s="16"/>

</xml_diff>

<commit_message>
update tutor records and finish exercise 2.77 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -224,7 +224,7 @@
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
 精锐教育是当月15号；星期天培训下个月20号；掌学教育是下月15号
 下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100
-李梦媛10月12日只上了半节课，唐润宁11月2日只上了半节课</t>
+李梦媛10月12日只上了半节课</t>
   </si>
   <si>
     <t>第11课</t>
@@ -1103,7 +1103,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1172,6 +1172,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1494,7 +1495,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1804,15 +1805,15 @@
       <c r="O6" s="9">
         <v>45592</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="9">
         <v>45599</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="9">
         <v>45606</v>
       </c>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
     </row>
     <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
finish exercise 2.78-2.80 of sicp
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -191,36 +191,6 @@
     <t>110/150</t>
   </si>
   <si>
-    <t>豌豆文化</t>
-  </si>
-  <si>
-    <t>周六17：10-19：10</t>
-  </si>
-  <si>
-    <t>孙朝(zhao)阳</t>
-  </si>
-  <si>
-    <t>天章大厦</t>
-  </si>
-  <si>
-    <t>60/100</t>
-  </si>
-  <si>
-    <t>450/2h</t>
-  </si>
-  <si>
-    <t>魏子骞</t>
-  </si>
-  <si>
-    <t>幸福路48号二建小区 9-2-302</t>
-  </si>
-  <si>
-    <t>13中</t>
-  </si>
-  <si>
-    <t>70/90</t>
-  </si>
-  <si>
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
 精锐教育是当月15号；星期天培训下个月20号；掌学教育是下月15号
 下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100
@@ -251,6 +221,9 @@
     <t>初二</t>
   </si>
   <si>
+    <t>豌豆文化</t>
+  </si>
+  <si>
     <t>260/2h</t>
   </si>
   <si>
@@ -302,6 +275,9 @@
     <t>德泽园三区1-1-202</t>
   </si>
   <si>
+    <t>60/100</t>
+  </si>
+  <si>
     <t>一尔优教育</t>
   </si>
   <si>
@@ -353,6 +329,9 @@
     <t>邮区中心局小区3-4-602</t>
   </si>
   <si>
+    <t>13中</t>
+  </si>
+  <si>
     <t>李冰惠</t>
   </si>
   <si>
@@ -368,6 +347,9 @@
     <t>夏锦程</t>
   </si>
   <si>
+    <t>天章大厦</t>
+  </si>
+  <si>
     <t>19中</t>
   </si>
   <si>
@@ -444,6 +426,24 @@
   </si>
   <si>
     <t>60/150</t>
+  </si>
+  <si>
+    <t>周六17：10-19：10</t>
+  </si>
+  <si>
+    <t>孙朝(zhao)阳</t>
+  </si>
+  <si>
+    <t>450/2h</t>
+  </si>
+  <si>
+    <t>魏子骞</t>
+  </si>
+  <si>
+    <t>幸福路48号二建小区 9-2-302</t>
+  </si>
+  <si>
+    <t>70/90</t>
   </si>
   <si>
     <t xml:space="preserve">绿色表示课时费已发；
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1959,102 +1959,8 @@
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="12">
-        <v>45430</v>
-      </c>
-      <c r="L10" s="12">
-        <v>45437</v>
-      </c>
-      <c r="M10" s="12">
-        <v>45451</v>
-      </c>
-      <c r="N10" s="12">
-        <v>45458</v>
-      </c>
-      <c r="O10" s="12">
-        <v>45465</v>
-      </c>
-      <c r="P10" s="9">
-        <v>45572</v>
-      </c>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-    </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:18">
-      <c r="A11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="12">
-        <v>45552</v>
-      </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-    </row>
+    <row r="10" customFormat="1"/>
+    <row r="11" customFormat="1"/>
     <row r="13" s="20" customFormat="1" ht="15.5"/>
     <row r="14" s="20" customFormat="1" ht="15.5"/>
     <row r="15" s="20" customFormat="1" ht="15.5"/>
@@ -2084,7 +1990,7 @@
     </row>
     <row r="20" ht="17.5" spans="2:13">
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2187,8 +2093,8 @@
   <sheetPr/>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2268,7 +2174,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="15.5" spans="1:21">
@@ -2279,25 +2185,25 @@
         <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J2" s="9">
         <v>45185</v>
@@ -2338,31 +2244,31 @@
     </row>
     <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>22</v>
@@ -2403,25 +2309,25 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -2438,25 +2344,25 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>22</v>
@@ -2492,31 +2398,31 @@
     </row>
     <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="J6" s="9">
         <v>45320</v>
@@ -2560,25 +2466,25 @@
         <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>22</v>
@@ -2606,25 +2512,25 @@
         <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2647,25 +2553,25 @@
         <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2817,25 +2723,25 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>22</v>
@@ -2903,25 +2809,25 @@
         <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>22</v>
@@ -2959,22 +2865,22 @@
         <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>52</v>
@@ -3021,25 +2927,25 @@
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>22</v>
@@ -3115,22 +3021,22 @@
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>28</v>
@@ -3209,25 +3115,25 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>22</v>
@@ -3345,25 +3251,25 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>22</v>
@@ -3487,25 +3393,25 @@
         <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="J27" s="12">
         <v>45451</v>
@@ -3531,31 +3437,31 @@
     </row>
     <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>22</v>
@@ -3573,27 +3479,101 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="30" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
+    <row r="29" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="12">
+        <v>45430</v>
+      </c>
+      <c r="L29" s="12">
+        <v>45437</v>
+      </c>
+      <c r="M29" s="12">
+        <v>45451</v>
+      </c>
+      <c r="N29" s="12">
+        <v>45458</v>
+      </c>
+      <c r="O29" s="12">
+        <v>45465</v>
+      </c>
+      <c r="P29" s="9">
+        <v>45572</v>
+      </c>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" customFormat="1" ht="15.5" spans="1:18">
+      <c r="A30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="12">
+        <v>45552</v>
+      </c>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
     </row>
     <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="4"/>

</xml_diff>

<commit_message>
finish exercise 2.81 of sicp and update tutor records
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -104,15 +104,81 @@
     <t>70/150</t>
   </si>
   <si>
+    <t>270/2h</t>
+  </si>
+  <si>
+    <t>周日11：00-13：00</t>
+  </si>
+  <si>
+    <t>刘桐语</t>
+  </si>
+  <si>
+    <t>莲湖路196号博香苑小区 6-2-1001</t>
+  </si>
+  <si>
+    <t>126中学</t>
+  </si>
+  <si>
+    <t>130/150</t>
+  </si>
+  <si>
+    <t>周日14：00-16：00</t>
+  </si>
+  <si>
+    <t>贾梦垚</t>
+  </si>
+  <si>
+    <t>莲湖路196号博香苑小区6-2-1001</t>
+  </si>
+  <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <t>星期天培训</t>
+  </si>
+  <si>
+    <t>周日17：00-19：00</t>
+  </si>
+  <si>
+    <t>李梦媛</t>
+  </si>
+  <si>
+    <t>南纬一路144号晟和家园 3-2203</t>
+  </si>
+  <si>
+    <t>70中</t>
+  </si>
+  <si>
+    <t>30/90</t>
+  </si>
+  <si>
+    <t>精锐教育</t>
+  </si>
+  <si>
+    <t>220/2h</t>
+  </si>
+  <si>
+    <t>周日20：00-22：00</t>
+  </si>
+  <si>
+    <t>孙翊原</t>
+  </si>
+  <si>
+    <t>卫生巷88号 6-1-403</t>
+  </si>
+  <si>
+    <t>兵一</t>
+  </si>
+  <si>
+    <t>110/150</t>
+  </si>
+  <si>
     <t>初一</t>
   </si>
   <si>
     <t>掌学教育</t>
   </si>
   <si>
-    <t>220/2h</t>
-  </si>
-  <si>
     <t>周六18：30-20：30</t>
   </si>
   <si>
@@ -122,79 +188,12 @@
     <t>新民路29号 3-201</t>
   </si>
   <si>
-    <t>兵一</t>
-  </si>
-  <si>
     <t>90/100</t>
-  </si>
-  <si>
-    <t>270/2h</t>
-  </si>
-  <si>
-    <t>周日11：00-13：00</t>
-  </si>
-  <si>
-    <t>刘桐语</t>
-  </si>
-  <si>
-    <t>莲湖路196号博香苑小区 6-2-1001</t>
-  </si>
-  <si>
-    <t>126中学</t>
-  </si>
-  <si>
-    <t>130/150</t>
-  </si>
-  <si>
-    <t>周日14：00-16：00</t>
-  </si>
-  <si>
-    <t>贾梦垚</t>
-  </si>
-  <si>
-    <t>莲湖路196号博香苑小区6-2-1001</t>
-  </si>
-  <si>
-    <t>物理</t>
-  </si>
-  <si>
-    <t>星期天培训</t>
-  </si>
-  <si>
-    <t>周日17：00-19：00</t>
-  </si>
-  <si>
-    <t>李梦媛</t>
-  </si>
-  <si>
-    <t>南纬一路144号晟和家园 3-2203</t>
-  </si>
-  <si>
-    <t>70中</t>
-  </si>
-  <si>
-    <t>30/90</t>
-  </si>
-  <si>
-    <t>精锐教育</t>
-  </si>
-  <si>
-    <t>周日20：00-22：00</t>
-  </si>
-  <si>
-    <t>孙翊原</t>
-  </si>
-  <si>
-    <t>卫生巷88号 6-1-403</t>
-  </si>
-  <si>
-    <t>110/150</t>
   </si>
   <si>
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
 精锐教育是当月15号；星期天培训下个月20号；掌学教育是下月15号
-下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100
-李梦媛10月12日只上了半节课</t>
+下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，唐润宁：100</t>
   </si>
   <si>
     <t>第11课</t>
@@ -1495,7 +1494,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1507,7 +1506,8 @@
     <col min="6" max="6" width="12.375" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="10" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="9.125" customWidth="1"/>
+    <col min="10" max="10" width="8.08333333333333" customWidth="1"/>
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1622,290 +1622,294 @@
       <c r="P2" s="21">
         <v>45605</v>
       </c>
-      <c r="Q2" s="20"/>
+      <c r="Q2" s="21">
+        <v>45612</v>
+      </c>
       <c r="R2" s="20"/>
     </row>
     <row r="3" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="9">
-        <v>45543</v>
-      </c>
-      <c r="K3" s="9">
-        <v>45550</v>
+      <c r="J3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12">
+        <v>45551</v>
       </c>
       <c r="L3" s="9">
         <v>45557</v>
       </c>
       <c r="M3" s="9">
+        <v>45563</v>
+      </c>
+      <c r="N3" s="9">
+        <v>45567</v>
+      </c>
+      <c r="O3" s="9">
         <v>45578</v>
       </c>
-      <c r="N3" s="9">
-        <v>45584</v>
-      </c>
-      <c r="O3" s="9">
-        <v>45591</v>
-      </c>
-      <c r="P3" s="21">
-        <v>45598</v>
-      </c>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
+      <c r="P3" s="9">
+        <v>45585</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>45592</v>
+      </c>
+      <c r="R3" s="9">
+        <v>45599</v>
+      </c>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
     </row>
     <row r="4" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+    </row>
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="9">
+        <v>45557</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45566</v>
+      </c>
+      <c r="M5" s="9">
+        <v>45572</v>
+      </c>
+      <c r="N5" s="9">
+        <v>45585</v>
+      </c>
+      <c r="O5" s="9">
+        <v>45592</v>
+      </c>
+      <c r="P5" s="9">
+        <v>45599</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>45606</v>
+      </c>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+    </row>
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="H6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K6" s="9">
         <v>45551</v>
       </c>
-      <c r="L4" s="9">
-        <v>45557</v>
-      </c>
-      <c r="M4" s="9">
+      <c r="L6" s="9">
+        <v>45556</v>
+      </c>
+      <c r="M6" s="9">
         <v>45563</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N6" s="9">
+        <v>45566</v>
+      </c>
+      <c r="O6" s="9">
         <v>45567</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P6" s="9">
+        <v>45572</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>45577</v>
+      </c>
+      <c r="R6" s="9">
         <v>45578</v>
       </c>
-      <c r="P4" s="9">
+      <c r="S6" s="9">
         <v>45585</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="T6" s="9">
         <v>45592</v>
       </c>
-      <c r="R4" s="9">
+    </row>
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="21">
         <v>45599</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-    </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-    </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A6" s="5" t="s">
+      <c r="L7" s="21">
+        <v>45606</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+    </row>
+    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="9">
-        <v>45557</v>
-      </c>
-      <c r="L6" s="9">
+      <c r="K8" s="12">
+        <v>45543</v>
+      </c>
+      <c r="L8" s="9">
         <v>45566</v>
       </c>
-      <c r="M6" s="9">
-        <v>45572</v>
-      </c>
-      <c r="N6" s="9">
+      <c r="M8" s="9">
+        <v>45567</v>
+      </c>
+      <c r="N8" s="9">
         <v>45585</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O8" s="9">
         <v>45592</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P8" s="9">
         <v>45599</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q8" s="9">
         <v>45606</v>
       </c>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-    </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="9">
-        <v>45551</v>
-      </c>
-      <c r="L7" s="9">
-        <v>45556</v>
-      </c>
-      <c r="M7" s="9">
-        <v>45563</v>
-      </c>
-      <c r="N7" s="21">
-        <v>45566</v>
-      </c>
-      <c r="O7" s="21">
-        <v>45567</v>
-      </c>
-      <c r="P7" s="21">
-        <v>45572</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>45577</v>
-      </c>
-      <c r="R7" s="21">
-        <v>45578</v>
-      </c>
-      <c r="S7" s="21">
-        <v>45585</v>
-      </c>
-      <c r="T7" s="21">
-        <v>45592</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="21">
-        <v>45599</v>
-      </c>
-      <c r="L8" s="21">
-        <v>45606</v>
-      </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
     </row>
     <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="5" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>21</v>
@@ -1914,7 +1918,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>54</v>
@@ -1926,41 +1930,37 @@
         <v>56</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="12">
+      <c r="J9" s="9">
         <v>45543</v>
       </c>
+      <c r="K9" s="9">
+        <v>45550</v>
+      </c>
       <c r="L9" s="9">
-        <v>45566</v>
+        <v>45557</v>
       </c>
       <c r="M9" s="9">
-        <v>45567</v>
+        <v>45578</v>
       </c>
       <c r="N9" s="9">
-        <v>45585</v>
+        <v>45584</v>
       </c>
       <c r="O9" s="9">
-        <v>45592</v>
+        <v>45591</v>
       </c>
       <c r="P9" s="21">
-        <v>45599</v>
-      </c>
-      <c r="Q9" s="21">
-        <v>45606</v>
-      </c>
-      <c r="R9" s="21"/>
+        <v>45598</v>
+      </c>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
     </row>
-    <row r="10" customFormat="1"/>
-    <row r="11" customFormat="1"/>
     <row r="13" s="20" customFormat="1" ht="15.5"/>
     <row r="14" s="20" customFormat="1" ht="15.5"/>
     <row r="15" s="20" customFormat="1" ht="15.5"/>
@@ -2060,26 +2060,26 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J6:J7"/>
     <mergeCell ref="B20:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2200,7 +2200,7 @@
         <v>64</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>65</v>
@@ -2359,7 +2359,7 @@
         <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>65</v>
@@ -2419,7 +2419,7 @@
         <v>84</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>85</v>
@@ -2481,7 +2481,7 @@
         <v>89</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>90</v>
@@ -2550,7 +2550,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>86</v>
@@ -2568,7 +2568,7 @@
         <v>98</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>99</v>
@@ -2824,7 +2824,7 @@
         <v>105</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>106</v>
@@ -2862,7 +2862,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>67</v>
@@ -2883,7 +2883,7 @@
         <v>110</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>22</v>
@@ -3390,7 +3390,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>86</v>
@@ -3484,7 +3484,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>67</v>
@@ -3502,7 +3502,7 @@
         <v>109</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>85</v>
@@ -3538,7 +3538,7 @@
         <v>20</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>22</v>
@@ -3547,7 +3547,7 @@
         <v>138</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
update tutor records and write diary
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -1109,7 +1109,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1174,16 +1174,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1509,7 +1504,7 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1664,15 +1659,17 @@
       <c r="K3" s="21">
         <v>45633</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="L3" s="21">
+        <v>45641</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
     </row>
     <row r="4" customFormat="1" ht="15.5" spans="1:20">
       <c r="A4" s="4" t="s">
@@ -1750,12 +1747,13 @@
       <c r="K5" s="9">
         <v>45627</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
     </row>
@@ -1965,10 +1963,10 @@
       <c r="Q9" s="9">
         <v>45606</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="10">
         <v>45613</v>
       </c>
-      <c r="S9" s="21">
+      <c r="S9" s="10">
         <v>45620</v>
       </c>
       <c r="T9" s="21">

</xml_diff>

<commit_message>
write diary and update tutor records
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -152,31 +152,10 @@
     <t>30/90</t>
   </si>
   <si>
-    <t>精锐教育</t>
-  </si>
-  <si>
-    <t>220/2h</t>
-  </si>
-  <si>
-    <t>周日20：00-22：00</t>
-  </si>
-  <si>
-    <t>孙翊原</t>
-  </si>
-  <si>
-    <t>卫生巷88号 6-1-403</t>
-  </si>
-  <si>
-    <t>兵一</t>
-  </si>
-  <si>
-    <t>110/150</t>
-  </si>
-  <si>
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：豌豆文化每月10号；
 精锐教育是当月15号；星期天培训下个月20号
 郭润宁11月19、27日上了半节课
-下次考试目标：刘桐语：135，李梦媛：50，孙翊原：120,贾梦垚：130，郭润宁：100</t>
+下次考试目标：刘桐语：135，李梦媛：50，贾梦垚：130，郭润宁：100</t>
   </si>
   <si>
     <t>第11课</t>
@@ -197,6 +176,9 @@
     <t>光明路北小区14-2-503</t>
   </si>
   <si>
+    <t>兵一</t>
+  </si>
+  <si>
     <t>90/150</t>
   </si>
   <si>
@@ -437,6 +419,9 @@
     <t>掌学教育</t>
   </si>
   <si>
+    <t>220/2h</t>
+  </si>
+  <si>
     <t>朱思臣</t>
   </si>
   <si>
@@ -444,6 +429,21 @@
   </si>
   <si>
     <t>90/100</t>
+  </si>
+  <si>
+    <t>精锐教育</t>
+  </si>
+  <si>
+    <t>周日20：00-22：00</t>
+  </si>
+  <si>
+    <t>孙翊原</t>
+  </si>
+  <si>
+    <t>卫生巷88号 6-1-403</t>
+  </si>
+  <si>
+    <t>110/150</t>
   </si>
   <si>
     <t xml:space="preserve">绿色表示课时费已发；
@@ -1174,7 +1174,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1501,10 +1503,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1660,7 +1662,7 @@
         <v>45633</v>
       </c>
       <c r="L3" s="21">
-        <v>45641</v>
+        <v>45640</v>
       </c>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
@@ -1747,7 +1749,9 @@
       <c r="K5" s="9">
         <v>45627</v>
       </c>
-      <c r="L5" s="24"/>
+      <c r="L5" s="9">
+        <v>45641</v>
+      </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
@@ -1758,19 +1762,19 @@
       <c r="T5" s="21"/>
     </row>
     <row r="6" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1779,7 +1783,7 @@
       <c r="G6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -1820,175 +1824,129 @@
       </c>
     </row>
     <row r="7" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="21">
+        <v>45641</v>
+      </c>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+    </row>
+    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K8" s="9">
         <v>45551</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L8" s="9">
         <v>45556</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M8" s="9">
         <v>45563</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N8" s="9">
         <v>45566</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O8" s="9">
         <v>45567</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P8" s="9">
         <v>45572</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="Q8" s="9">
         <v>45577</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R8" s="9">
         <v>45578</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S8" s="9">
         <v>45585</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T8" s="9">
         <v>45592</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="21">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="21">
         <v>45599</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L9" s="21">
         <v>45606</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M9" s="21">
         <v>45613</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N9" s="21">
         <v>45627</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-    </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="12">
-        <v>45543</v>
-      </c>
-      <c r="L9" s="9">
-        <v>45566</v>
-      </c>
-      <c r="M9" s="9">
-        <v>45567</v>
-      </c>
-      <c r="N9" s="9">
-        <v>45585</v>
-      </c>
-      <c r="O9" s="9">
-        <v>45592</v>
-      </c>
-      <c r="P9" s="9">
-        <v>45599</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>45606</v>
-      </c>
-      <c r="R9" s="10">
-        <v>45613</v>
-      </c>
-      <c r="S9" s="10">
-        <v>45620</v>
-      </c>
-      <c r="T9" s="21">
-        <v>45627</v>
-      </c>
-    </row>
-    <row r="14" s="20" customFormat="1" ht="15.5"/>
+      <c r="O9" s="21">
+        <v>45641</v>
+      </c>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+    </row>
+    <row r="10" customFormat="1"/>
     <row r="15" s="20" customFormat="1" ht="15.5"/>
     <row r="16" s="20" customFormat="1" ht="15.5"/>
     <row r="17" s="20" customFormat="1" ht="15.5"/>
     <row r="18" s="20" customFormat="1" ht="15.5"/>
-    <row r="19" s="20" customFormat="1" ht="15.5" spans="1:9">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-    </row>
+    <row r="19" s="20" customFormat="1" ht="15.5"/>
     <row r="20" s="20" customFormat="1" ht="15.5" spans="1:9">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
@@ -2000,24 +1958,21 @@
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" ht="17.5" spans="2:13">
-      <c r="B21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
+    <row r="21" s="20" customFormat="1" ht="15.5" spans="1:9">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" ht="17.5" spans="2:13">
-      <c r="B22" s="8"/>
+      <c r="B22" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2030,7 +1985,7 @@
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
     </row>
-    <row r="23" ht="17.5" spans="2:12">
+    <row r="23" ht="17.5" spans="2:13">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2039,10 +1994,12 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="25"/>
       <c r="L23" s="25"/>
-    </row>
-    <row r="24" ht="17.5" spans="2:13">
+      <c r="M23" s="25"/>
+    </row>
+    <row r="24" ht="17.5" spans="2:12">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2051,10 +2008,8 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="25"/>
       <c r="K24" s="25"/>
       <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
     </row>
     <row r="25" ht="17.5" spans="2:13">
       <c r="B25" s="8"/>
@@ -2070,39 +2025,62 @@
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
     </row>
+    <row r="26" ht="17.5" spans="2:13">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="40">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="B21:I25"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B22:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2113,10 +2091,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2196,7 +2174,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="15.5" spans="1:21">
@@ -2207,25 +2185,25 @@
         <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J2" s="9">
         <v>45185</v>
@@ -2266,31 +2244,31 @@
     </row>
     <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>22</v>
@@ -2331,25 +2309,25 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J4" s="9">
         <v>45287</v>
@@ -2366,25 +2344,25 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>22</v>
@@ -2420,31 +2398,31 @@
     </row>
     <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J6" s="9">
         <v>45320</v>
@@ -2488,25 +2466,25 @@
         <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>22</v>
@@ -2534,25 +2512,25 @@
         <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J8" s="14">
         <v>45425</v>
@@ -2575,25 +2553,25 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="J9" s="9">
         <v>45186</v>
@@ -2745,25 +2723,25 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>22</v>
@@ -2831,25 +2809,25 @@
         <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>22</v>
@@ -2887,22 +2865,22 @@
         <v>38</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>44</v>
@@ -2949,25 +2927,25 @@
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>22</v>
@@ -3043,22 +3021,22 @@
         <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>28</v>
@@ -3137,25 +3115,25 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>22</v>
@@ -3273,25 +3251,25 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>22</v>
@@ -3415,25 +3393,25 @@
         <v>38</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J27" s="12">
         <v>45451</v>
@@ -3459,31 +3437,31 @@
     </row>
     <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>22</v>
@@ -3509,25 +3487,25 @@
         <v>38</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J29" s="12" t="s">
         <v>22</v>
@@ -3566,22 +3544,22 @@
         <v>22</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>22</v>
@@ -3599,31 +3577,31 @@
     </row>
     <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J31" s="9">
         <v>45543</v>
@@ -3652,26 +3630,66 @@
       <c r="T31" s="20"/>
     </row>
     <row r="32" customFormat="1" ht="15.5" spans="1:20">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
+      <c r="A32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="12">
+        <v>45543</v>
+      </c>
+      <c r="L32" s="9">
+        <v>45566</v>
+      </c>
+      <c r="M32" s="9">
+        <v>45567</v>
+      </c>
+      <c r="N32" s="9">
+        <v>45585</v>
+      </c>
+      <c r="O32" s="9">
+        <v>45592</v>
+      </c>
+      <c r="P32" s="9">
+        <v>45599</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>45606</v>
+      </c>
+      <c r="R32" s="10">
+        <v>45613</v>
+      </c>
+      <c r="S32" s="10">
+        <v>45620</v>
+      </c>
+      <c r="T32" s="9">
+        <v>45627</v>
+      </c>
     </row>
     <row r="33" customFormat="1" ht="15.5" spans="1:20">
       <c r="A33" s="4"/>
@@ -3805,22 +3823,32 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
     </row>
-    <row r="39" spans="2:11">
-      <c r="B39" s="8" t="s">
+    <row r="39" customFormat="1" ht="15.5" spans="1:20">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-    </row>
-    <row r="40" spans="2:11">
-      <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
@@ -3890,6 +3918,18 @@
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="61">
@@ -3953,7 +3993,7 @@
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="J24:J26"/>
-    <mergeCell ref="B39:K45"/>
+    <mergeCell ref="B40:K46"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add a book of positive psychology
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -161,8 +161,8 @@
     <t>30/90</t>
   </si>
   <si>
-    <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：精锐教育是当月15号；
-星期天培训下个月20号;郭润宁11月19、27日上了半节课
+    <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：
+精锐教育是当月15号；星期天培训下个月20号;
 下次考试目标：刘桐语：135，李梦媛：50，贾梦垚：130，郭润宁：100</t>
   </si>
   <si>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1619,7 +1619,9 @@
       <c r="M2" s="21">
         <v>45650</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="21">
+        <v>45653</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>

</xml_diff>

<commit_message>
del useless files and learn big data
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -463,10 +463,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -964,7 +964,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -973,10 +973,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -985,7 +985,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1503,10 +1503,10 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -1520,7 +1520,7 @@
     <col min="11" max="20" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:20">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:20">
+    <row r="2" customFormat="1" ht="15.75" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:20">
+    <row r="3" customFormat="1" ht="15.75" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:20">
+    <row r="4" customFormat="1" ht="15.75" spans="1:20">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1721,16 +1721,16 @@
       <c r="L4" s="9">
         <v>45640</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="9">
         <v>45647</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="9">
         <v>45654</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="9">
         <v>45661</v>
       </c>
-      <c r="P4" s="21">
+      <c r="P4" s="9">
         <v>45668</v>
       </c>
       <c r="Q4" s="21"/>
@@ -1738,7 +1738,7 @@
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1832,7 +1832,7 @@
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+    <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1905,13 +1905,13 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="21">
+      <c r="K8" s="9">
         <v>45641</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="9">
         <v>45648</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="9">
         <v>45662</v>
       </c>
       <c r="N8" s="21"/>
@@ -1922,7 +1922,7 @@
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="T10" s="20"/>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -2076,12 +2076,12 @@
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
     </row>
-    <row r="17" s="20" customFormat="1" ht="15.5"/>
-    <row r="18" s="20" customFormat="1" ht="15.5"/>
-    <row r="19" s="20" customFormat="1" ht="15.5"/>
-    <row r="20" s="20" customFormat="1" ht="15.5"/>
-    <row r="21" s="20" customFormat="1" ht="15.5"/>
-    <row r="22" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="17" s="20" customFormat="1" ht="15.75"/>
+    <row r="18" s="20" customFormat="1" ht="15.75"/>
+    <row r="19" s="20" customFormat="1" ht="15.75"/>
+    <row r="20" s="20" customFormat="1" ht="15.75"/>
+    <row r="21" s="20" customFormat="1" ht="15.75"/>
+    <row r="22" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -2092,7 +2092,7 @@
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="23" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2103,7 +2103,7 @@
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
     </row>
-    <row r="24" ht="17.5" spans="2:13">
+    <row r="24" ht="18.75" spans="2:13">
       <c r="B24" s="8" t="s">
         <v>54</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
     </row>
-    <row r="25" ht="17.5" spans="2:13">
+    <row r="25" ht="18.75" spans="2:13">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -2133,7 +2133,7 @@
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
     </row>
-    <row r="26" ht="17.5" spans="2:12">
+    <row r="26" ht="18.75" spans="2:12">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -2145,7 +2145,7 @@
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
     </row>
-    <row r="27" ht="17.5" spans="2:13">
+    <row r="27" ht="18.75" spans="2:13">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2159,7 +2159,7 @@
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
     </row>
-    <row r="28" ht="17.5" spans="2:13">
+    <row r="28" ht="18.75" spans="2:13">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2231,7 +2231,7 @@
       <selection activeCell="A27" sqref="$A27:$XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2246,7 +2246,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:21">
+    <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:19">
+    <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:11">
+    <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>63</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2679,7 +2679,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2783,7 +2783,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2825,7 +2825,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.5" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2849,7 +2849,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.5" spans="1:20">
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.5" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2935,7 +2935,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.5" spans="1:20">
+    <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2991,7 +2991,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.5" spans="1:20">
+    <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.5" spans="1:20">
+    <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.5" spans="1:20">
+    <row r="18" customFormat="1" ht="15.75" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3147,7 +3147,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.5" spans="1:20">
+    <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.5" spans="1:20">
+    <row r="20" customFormat="1" ht="15.75" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3241,7 +3241,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.5" spans="1:20">
+    <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.5" spans="1:20">
+    <row r="22" customFormat="1" ht="15.75" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3345,7 +3345,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.5" spans="1:20">
+    <row r="23" customFormat="1" ht="15.75" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3377,7 +3377,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.5" spans="1:20">
+    <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.5" spans="1:20">
+    <row r="25" customFormat="1" ht="15.75" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3481,7 +3481,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3519,7 +3519,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="28" customFormat="1" ht="15.5" spans="1:20">
+    <row r="28" customFormat="1" ht="15.75" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>121</v>
       </c>
@@ -3563,7 +3563,7 @@
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
     </row>
-    <row r="29" customFormat="1" ht="15.5" spans="1:20">
+    <row r="29" customFormat="1" ht="15.75" spans="1:20">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -3617,7 +3617,7 @@
       <c r="S29" s="16"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" customFormat="1" ht="15.5" spans="1:18">
+    <row r="30" customFormat="1" ht="15.75" spans="1:18">
       <c r="A30" s="5" t="s">
         <v>20</v>
       </c>
@@ -3659,7 +3659,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" customFormat="1" ht="15.5" spans="1:20">
+    <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>133</v>
       </c>
@@ -3713,7 +3713,7 @@
       <c r="S31" s="20"/>
       <c r="T31" s="20"/>
     </row>
-    <row r="32" customFormat="1" ht="15.5" spans="1:20">
+    <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.5" spans="1:20">
+    <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3797,7 +3797,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.5" spans="1:20">
+    <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3819,7 +3819,7 @@
       <c r="S34" s="22"/>
       <c r="T34" s="22"/>
     </row>
-    <row r="35" customFormat="1" ht="15.5" spans="1:20">
+    <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3841,7 +3841,7 @@
       <c r="S35" s="22"/>
       <c r="T35" s="22"/>
     </row>
-    <row r="36" customFormat="1" ht="15.5" spans="1:20">
+    <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -3863,7 +3863,7 @@
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
     </row>
-    <row r="37" customFormat="1" ht="15.5" spans="1:20">
+    <row r="37" customFormat="1" ht="15.75" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -3885,7 +3885,7 @@
       <c r="S37" s="22"/>
       <c r="T37" s="22"/>
     </row>
-    <row r="38" customFormat="1" ht="15.5" spans="1:20">
+    <row r="38" customFormat="1" ht="15.75" spans="1:20">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -3907,7 +3907,7 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
     </row>
-    <row r="39" customFormat="1" ht="15.5" spans="1:20">
+    <row r="39" customFormat="1" ht="15.75" spans="1:20">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>

</xml_diff>

<commit_message>
write diary and update tutor record
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -1509,7 +1509,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1712,7 +1712,9 @@
       <c r="M4" s="21">
         <v>45694</v>
       </c>
-      <c r="N4" s="21"/>
+      <c r="N4" s="21">
+        <v>45698</v>
+      </c>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>

</xml_diff>

<commit_message>
modify tasks and update tutor records
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -89,13 +89,13 @@
     <t>270/1.5h</t>
   </si>
   <si>
-    <t>周一、二、五21：00-22：30</t>
+    <t>周一、二、五 21：00-22：30</t>
   </si>
   <si>
     <t>李梦媛</t>
   </si>
   <si>
-    <t>南纬一路144号晟和家园 3-2203</t>
+    <t>晟和家园 3-2203</t>
   </si>
   <si>
     <t>70中</t>
@@ -113,7 +113,7 @@
     <t>郭润宁</t>
   </si>
   <si>
-    <t>西山东街261号 华美·博奥小区 7-3-401</t>
+    <t>嘉和苑·悦园 3楼</t>
   </si>
   <si>
     <t>13中分校</t>
@@ -131,7 +131,7 @@
     <t>刘桐语</t>
   </si>
   <si>
-    <t>莲湖路196号博香苑小区 6-2-1001</t>
+    <t>博香苑A区 6-2-1001</t>
   </si>
   <si>
     <t>126中学</t>
@@ -146,7 +146,7 @@
     <t>贾梦垚</t>
   </si>
   <si>
-    <t>莲湖路196号博香苑小区6-2-1001</t>
+    <t>德泽园3区1-1-101</t>
   </si>
   <si>
     <t>物理</t>
@@ -162,7 +162,7 @@
   </si>
   <si>
     <t>转账时间(灰色表示线上上课（课时费1小时100），绿色表示课时费已发)：
-精锐教育是当月15号；星期天培训下个月20号;2月2日至2月7日，李梦媛每天上了2小时
+精锐教育是当月15号；星期天培训下个月20号;2月2日至2月6日，2月10日至2月14日，李梦媛每天上了2小时
 下次考试目标：刘桐语：135，李梦媛：数学90物理50，贾梦垚：130，郭润宁：100</t>
   </si>
   <si>
@@ -1519,8 +1519,8 @@
   <sheetPr/>
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1528,9 +1528,9 @@
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="7.83333333333333" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
+    <col min="5" max="5" width="26.75" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="18.75" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
@@ -1732,7 +1732,9 @@
       <c r="P4" s="26">
         <v>45700</v>
       </c>
-      <c r="Q4" s="26"/>
+      <c r="Q4" s="26">
+        <v>45701</v>
+      </c>
       <c r="R4" s="26"/>
       <c r="S4" s="26"/>
       <c r="T4" s="26"/>
@@ -2224,22 +2226,22 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D9:D10"/>

</xml_diff>

<commit_message>
add toc for one book
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -487,11 +487,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -989,7 +989,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -998,10 +998,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1010,7 +1010,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1134,7 +1134,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1190,10 +1190,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1208,16 +1208,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1539,11 +1536,11 @@
   <sheetPr/>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
@@ -1557,7 +1554,7 @@
     <col min="11" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:20">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1619,7 +1616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:20">
+    <row r="2" customFormat="1" ht="15.75" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:20">
+    <row r="3" customFormat="1" ht="15.75" spans="1:20">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1723,7 +1720,7 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:20">
+    <row r="4" customFormat="1" ht="15.75" spans="1:20">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1765,7 +1762,7 @@
         <v>45712</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1795,7 +1792,7 @@
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1857,7 +1854,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1899,7 +1896,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.5" spans="1:20">
+    <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1929,7 +1926,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1983,7 +1980,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2045,7 +2042,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2083,7 +2080,7 @@
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
     </row>
-    <row r="12" customFormat="1" ht="15.5" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2095,17 +2092,17 @@
       <c r="I12" s="4"/>
       <c r="J12" s="9"/>
       <c r="K12" s="21"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-    </row>
-    <row r="13" customFormat="1" ht="15.5" spans="1:20">
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+    </row>
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.5" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2199,22 +2196,37 @@
       <c r="Q14" s="21">
         <v>45655</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="21">
         <v>45662</v>
       </c>
-      <c r="S14" s="22">
+      <c r="S14" s="21">
         <v>45669</v>
       </c>
-      <c r="T14" s="22">
+      <c r="T14" s="21">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" spans="1:11">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="21">
         <v>45725</v>
       </c>
     </row>
-    <row r="22" s="20" customFormat="1" ht="15.5"/>
-    <row r="23" s="20" customFormat="1" ht="15.5"/>
-    <row r="24" s="20" customFormat="1" ht="15.5"/>
-    <row r="25" s="20" customFormat="1" ht="15.5"/>
-    <row r="26" s="20" customFormat="1" ht="15.5"/>
-    <row r="27" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="22" s="20" customFormat="1" ht="15.75"/>
+    <row r="23" s="20" customFormat="1" ht="15.75"/>
+    <row r="24" s="20" customFormat="1" ht="15.75"/>
+    <row r="25" s="20" customFormat="1" ht="15.75"/>
+    <row r="26" s="20" customFormat="1" ht="15.75"/>
+    <row r="27" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
@@ -2225,7 +2237,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" s="20" customFormat="1" ht="15.5" spans="1:9">
+    <row r="28" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A28" s="25"/>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -2236,7 +2248,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" ht="17.5" spans="2:13">
+    <row r="29" ht="18.75" spans="2:13">
       <c r="B29" s="8" t="s">
         <v>52</v>
       </c>
@@ -2247,12 +2259,12 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-    </row>
-    <row r="30" ht="17.5" spans="2:13">
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+    </row>
+    <row r="30" ht="18.75" spans="2:13">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2261,12 +2273,12 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-    </row>
-    <row r="31" ht="17.5" spans="2:12">
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+    </row>
+    <row r="31" ht="18.75" spans="2:12">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -2275,10 +2287,10 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-    </row>
-    <row r="32" ht="17.5" spans="2:13">
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" ht="18.75" spans="2:13">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -2287,12 +2299,12 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-    </row>
-    <row r="33" ht="17.5" spans="2:13">
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+    </row>
+    <row r="33" ht="18.75" spans="2:13">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -2301,53 +2313,53 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="41">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C13:C15"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D13:D15"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F13:F15"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G13:G15"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H13:H15"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="I10:I12"/>
-    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I13:I15"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J13:J15"/>
     <mergeCell ref="B29:I33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2365,7 +2377,7 @@
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2380,7 +2392,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.5" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.5" spans="1:21">
+    <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2510,7 +2522,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.5" spans="1:19">
+    <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
@@ -2569,7 +2581,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.5" spans="1:11">
+    <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2604,7 +2616,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.5" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2664,7 +2676,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.5" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
@@ -2726,7 +2738,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.5" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2813,7 +2825,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.5" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.5" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2917,7 +2929,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.5" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2959,7 +2971,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.5" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2983,7 +2995,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.5" spans="1:20">
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -3045,7 +3057,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.5" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3069,7 +3081,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.5" spans="1:20">
+    <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3125,7 +3137,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.5" spans="1:20">
+    <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.5" spans="1:20">
+    <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3249,7 +3261,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.5" spans="1:20">
+    <row r="18" customFormat="1" ht="15.75" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3281,7 +3293,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.5" spans="1:20">
+    <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3343,7 +3355,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.5" spans="1:20">
+    <row r="20" customFormat="1" ht="15.75" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3375,7 +3387,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.5" spans="1:20">
+    <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3437,7 +3449,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.5" spans="1:20">
+    <row r="22" customFormat="1" ht="15.75" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3479,7 +3491,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.5" spans="1:20">
+    <row r="23" customFormat="1" ht="15.75" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3511,7 +3523,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.5" spans="1:20">
+    <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3573,7 +3585,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.5" spans="1:20">
+    <row r="25" customFormat="1" ht="15.75" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3615,7 +3627,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3653,7 +3665,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.5" spans="1:20">
+    <row r="27" customFormat="1" ht="15.75" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>120</v>
       </c>
@@ -3697,7 +3709,7 @@
       <c r="S27" s="23"/>
       <c r="T27" s="23"/>
     </row>
-    <row r="28" customFormat="1" ht="15.5" spans="1:20">
+    <row r="28" customFormat="1" ht="15.75" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
@@ -3751,7 +3763,7 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15.5" spans="1:18">
+    <row r="29" customFormat="1" ht="15.75" spans="1:18">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -3793,7 +3805,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" customFormat="1" ht="15.5" spans="1:20">
+    <row r="30" customFormat="1" ht="15.75" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>133</v>
       </c>
@@ -3847,7 +3859,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
     </row>
-    <row r="31" customFormat="1" ht="15.5" spans="1:20">
+    <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
@@ -3909,7 +3921,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15.5" spans="1:20">
+    <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3971,7 +3983,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.5" spans="1:20">
+    <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3999,7 +4011,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.5" spans="1:20">
+    <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
@@ -4055,7 +4067,7 @@
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
     </row>
-    <row r="35" customFormat="1" ht="15.5" spans="1:20">
+    <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -4077,7 +4089,7 @@
       <c r="S35" s="24"/>
       <c r="T35" s="24"/>
     </row>
-    <row r="36" customFormat="1" ht="15.5" spans="1:20">
+    <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -4099,7 +4111,7 @@
       <c r="S36" s="24"/>
       <c r="T36" s="24"/>
     </row>
-    <row r="37" customFormat="1" ht="15.5" spans="1:20">
+    <row r="37" customFormat="1" ht="15.75" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -4121,7 +4133,7 @@
       <c r="S37" s="24"/>
       <c r="T37" s="24"/>
     </row>
-    <row r="38" customFormat="1" ht="15.5" spans="1:20">
+    <row r="38" customFormat="1" ht="15.75" spans="1:20">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4143,7 +4155,7 @@
       <c r="S38" s="24"/>
       <c r="T38" s="24"/>
     </row>
-    <row r="39" customFormat="1" ht="15.5" spans="1:20">
+    <row r="39" customFormat="1" ht="15.75" spans="1:20">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -4165,7 +4177,7 @@
       <c r="S39" s="24"/>
       <c r="T39" s="24"/>
     </row>
-    <row r="40" customFormat="1" ht="15.5" spans="1:20">
+    <row r="40" customFormat="1" ht="15.75" spans="1:20">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -4187,7 +4199,7 @@
       <c r="S40" s="24"/>
       <c r="T40" s="24"/>
     </row>
-    <row r="41" customFormat="1" ht="15.5" spans="1:20">
+    <row r="41" customFormat="1" ht="15.75" spans="1:20">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
Revert "add toc for one book"
This reverts commit 617ecca99b9543857b4675bbb5ac40218b8730e8.
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -487,11 +487,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -989,7 +989,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -998,10 +998,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1010,7 +1010,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1134,7 +1134,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1190,10 +1190,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1208,13 +1208,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1536,11 +1539,11 @@
   <sheetPr/>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
@@ -1554,7 +1557,7 @@
     <col min="11" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15.5" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:20">
+    <row r="2" customFormat="1" ht="15.5" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:20">
+    <row r="3" customFormat="1" ht="15.5" spans="1:20">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1720,7 +1723,7 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:20">
+    <row r="4" customFormat="1" ht="15.5" spans="1:20">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1762,7 +1765,7 @@
         <v>45712</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1792,7 +1795,7 @@
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1896,7 +1899,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.75" spans="1:20">
+    <row r="8" customFormat="1" ht="15.5" spans="1:20">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1926,7 +1929,7 @@
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1980,7 +1983,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15.5" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2080,7 +2083,7 @@
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15.5" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2092,17 +2095,17 @@
       <c r="I12" s="4"/>
       <c r="J12" s="9"/>
       <c r="K12" s="21"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+    </row>
+    <row r="13" customFormat="1" ht="15.5" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15.5" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2196,37 +2199,22 @@
       <c r="Q14" s="21">
         <v>45655</v>
       </c>
-      <c r="R14" s="21">
+      <c r="R14" s="22">
         <v>45662</v>
       </c>
-      <c r="S14" s="21">
+      <c r="S14" s="22">
         <v>45669</v>
       </c>
-      <c r="T14" s="21">
-        <v>45718</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" spans="1:11">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="21">
+      <c r="T14" s="22">
         <v>45725</v>
       </c>
     </row>
-    <row r="22" s="20" customFormat="1" ht="15.75"/>
-    <row r="23" s="20" customFormat="1" ht="15.75"/>
-    <row r="24" s="20" customFormat="1" ht="15.75"/>
-    <row r="25" s="20" customFormat="1" ht="15.75"/>
-    <row r="26" s="20" customFormat="1" ht="15.75"/>
-    <row r="27" s="20" customFormat="1" ht="15.75" spans="1:9">
+    <row r="22" s="20" customFormat="1" ht="15.5"/>
+    <row r="23" s="20" customFormat="1" ht="15.5"/>
+    <row r="24" s="20" customFormat="1" ht="15.5"/>
+    <row r="25" s="20" customFormat="1" ht="15.5"/>
+    <row r="26" s="20" customFormat="1" ht="15.5"/>
+    <row r="27" s="20" customFormat="1" ht="15.5" spans="1:9">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
@@ -2237,7 +2225,7 @@
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" s="20" customFormat="1" ht="15.75" spans="1:9">
+    <row r="28" s="20" customFormat="1" ht="15.5" spans="1:9">
       <c r="A28" s="25"/>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -2248,7 +2236,7 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" ht="18.75" spans="2:13">
+    <row r="29" ht="17.5" spans="2:13">
       <c r="B29" s="8" t="s">
         <v>52</v>
       </c>
@@ -2259,12 +2247,12 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-    </row>
-    <row r="30" ht="18.75" spans="2:13">
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+    </row>
+    <row r="30" ht="17.5" spans="2:13">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2273,12 +2261,12 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-    </row>
-    <row r="31" ht="18.75" spans="2:12">
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+    </row>
+    <row r="31" ht="17.5" spans="2:12">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -2287,10 +2275,10 @@
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-    </row>
-    <row r="32" ht="18.75" spans="2:13">
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+    </row>
+    <row r="32" ht="17.5" spans="2:13">
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -2299,12 +2287,12 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-    </row>
-    <row r="33" ht="18.75" spans="2:13">
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+    </row>
+    <row r="33" ht="17.5" spans="2:13">
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -2313,53 +2301,53 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="41">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H8"/>
     <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="H13:H14"/>
     <mergeCell ref="I2:I5"/>
     <mergeCell ref="I6:I8"/>
     <mergeCell ref="I10:I12"/>
-    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="J6:J8"/>
     <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="B29:I33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2377,7 +2365,7 @@
       <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
@@ -2392,7 +2380,7 @@
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15.5" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2445,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15.5" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2522,7 +2510,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15.5" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>61</v>
       </c>
@@ -2581,7 +2569,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15.5" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2616,7 +2604,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15.5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2676,7 +2664,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15.5" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
@@ -2738,7 +2726,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15.5" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2825,7 +2813,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15.5" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2887,7 +2875,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15.5" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2929,7 +2917,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15.5" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2971,7 +2959,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15.5" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2995,7 +2983,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15.5" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -3057,7 +3045,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15.5" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -3081,7 +3069,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15.5" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3137,7 +3125,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15.5" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3199,7 +3187,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15.5" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3261,7 +3249,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15.5" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3293,7 +3281,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15.5" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3355,7 +3343,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15.5" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3387,7 +3375,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15.5" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3449,7 +3437,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15.5" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3491,7 +3479,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15.5" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3523,7 +3511,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15.5" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3585,7 +3573,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15.5" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3627,7 +3615,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.5" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3665,7 +3653,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15.5" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>120</v>
       </c>
@@ -3709,7 +3697,7 @@
       <c r="S27" s="23"/>
       <c r="T27" s="23"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15.5" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
@@ -3763,7 +3751,7 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:18">
+    <row r="29" customFormat="1" ht="15.5" spans="1:18">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -3805,7 +3793,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15.5" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>133</v>
       </c>
@@ -3859,7 +3847,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15.5" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
@@ -3921,7 +3909,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15.5" spans="1:20">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3983,7 +3971,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15.5" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -4011,7 +3999,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15.5" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
@@ -4067,7 +4055,7 @@
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15.5" spans="1:20">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -4089,7 +4077,7 @@
       <c r="S35" s="24"/>
       <c r="T35" s="24"/>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15.5" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -4111,7 +4099,7 @@
       <c r="S36" s="24"/>
       <c r="T36" s="24"/>
     </row>
-    <row r="37" customFormat="1" ht="15.75" spans="1:20">
+    <row r="37" customFormat="1" ht="15.5" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -4133,7 +4121,7 @@
       <c r="S37" s="24"/>
       <c r="T37" s="24"/>
     </row>
-    <row r="38" customFormat="1" ht="15.75" spans="1:20">
+    <row r="38" customFormat="1" ht="15.5" spans="1:20">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4155,7 +4143,7 @@
       <c r="S38" s="24"/>
       <c r="T38" s="24"/>
     </row>
-    <row r="39" customFormat="1" ht="15.75" spans="1:20">
+    <row r="39" customFormat="1" ht="15.5" spans="1:20">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -4177,7 +4165,7 @@
       <c r="S39" s="24"/>
       <c r="T39" s="24"/>
     </row>
-    <row r="40" customFormat="1" ht="15.75" spans="1:20">
+    <row r="40" customFormat="1" ht="15.5" spans="1:20">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -4199,7 +4187,7 @@
       <c r="S40" s="24"/>
       <c r="T40" s="24"/>
     </row>
-    <row r="41" customFormat="1" ht="15.75" spans="1:20">
+    <row r="41" customFormat="1" ht="15.5" spans="1:20">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
finish reading Marva Collins' Way
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -491,11 +491,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -993,7 +993,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1002,10 +1002,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1014,7 +1014,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1194,10 +1194,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1212,13 +1212,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1541,24 +1541,24 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
-    <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
+    <col min="1" max="2" width="5.58181818181818" customWidth="1"/>
+    <col min="3" max="3" width="10.6636363636364" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="30.4583333333333" customWidth="1"/>
+    <col min="5" max="5" width="30.4545454545455" customWidth="1"/>
     <col min="6" max="6" width="7.5" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="9" width="9.125" customWidth="1"/>
-    <col min="10" max="10" width="10.8333333333333" customWidth="1"/>
+    <col min="8" max="8" width="9.87272727272727" customWidth="1"/>
+    <col min="9" max="9" width="9.12727272727273" customWidth="1"/>
+    <col min="10" max="10" width="10.8363636363636" customWidth="1"/>
     <col min="11" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:20">
+    <row r="2" customFormat="1" ht="15" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:20">
+    <row r="3" customFormat="1" ht="15" spans="1:20">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1724,7 +1724,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:20">
+    <row r="4" customFormat="1" ht="15" spans="1:20">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1753,12 +1753,14 @@
       <c r="P4" s="22">
         <v>45752</v>
       </c>
-      <c r="Q4" s="22"/>
+      <c r="Q4" s="22">
+        <v>45759</v>
+      </c>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1820,7 +1822,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15" spans="1:20">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1837,8 +1839,12 @@
       <c r="L6" s="22">
         <v>45753</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
+      <c r="M6" s="22">
+        <v>45759</v>
+      </c>
+      <c r="N6" s="22">
+        <v>45760</v>
+      </c>
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
@@ -1846,7 +1852,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.75" spans="1:20">
+    <row r="8" customFormat="1" ht="15" spans="1:20">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1950,7 +1956,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15" spans="1:20">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1964,7 +1970,9 @@
       <c r="K9" s="21">
         <v>45753</v>
       </c>
-      <c r="L9" s="22"/>
+      <c r="L9" s="22">
+        <v>45760</v>
+      </c>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
@@ -1974,7 +1982,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2036,7 +2044,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2078,7 +2086,7 @@
         <v>45718</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:13">
+    <row r="12" ht="15" spans="1:13">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2099,12 +2107,12 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="19" s="20" customFormat="1" ht="15.75"/>
-    <row r="20" s="20" customFormat="1" ht="15.75"/>
-    <row r="21" s="20" customFormat="1" ht="15.75"/>
-    <row r="22" s="20" customFormat="1" ht="15.75"/>
-    <row r="23" s="20" customFormat="1" ht="15.75"/>
-    <row r="24" s="20" customFormat="1" ht="15.75" spans="1:9">
+    <row r="19" s="20" customFormat="1" ht="15"/>
+    <row r="20" s="20" customFormat="1" ht="15"/>
+    <row r="21" s="20" customFormat="1" ht="15"/>
+    <row r="22" s="20" customFormat="1" ht="15"/>
+    <row r="23" s="20" customFormat="1" ht="15"/>
+    <row r="24" s="20" customFormat="1" ht="15" spans="1:9">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -2115,7 +2123,7 @@
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" s="20" customFormat="1" ht="15.75" spans="1:9">
+    <row r="25" s="20" customFormat="1" ht="15" spans="1:9">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -2126,7 +2134,7 @@
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" ht="18.75" spans="2:13">
+    <row r="26" ht="17.5" spans="2:13">
       <c r="B26" s="8" t="s">
         <v>49</v>
       </c>
@@ -2142,7 +2150,7 @@
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
     </row>
-    <row r="27" ht="18.75" spans="2:13">
+    <row r="27" ht="17.5" spans="2:13">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2156,7 +2164,7 @@
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
     </row>
-    <row r="28" ht="18.75" spans="2:12">
+    <row r="28" ht="17.5" spans="2:12">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2168,7 +2176,7 @@
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
     </row>
-    <row r="29" ht="18.75" spans="2:13">
+    <row r="29" ht="17.5" spans="2:13">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -2182,7 +2190,7 @@
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
     </row>
-    <row r="30" ht="18.75" spans="2:13">
+    <row r="30" ht="17.5" spans="2:13">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2255,22 +2263,22 @@
       <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="1" max="2" width="4.58181818181818" customWidth="1"/>
+    <col min="3" max="3" width="10.8727272727273" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="18.5833333333333" customWidth="1"/>
-    <col min="6" max="6" width="7.33333333333333" customWidth="1"/>
-    <col min="7" max="7" width="27.125" customWidth="1"/>
-    <col min="8" max="9" width="9.58333333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="18.5818181818182" customWidth="1"/>
+    <col min="6" max="6" width="7.33636363636364" customWidth="1"/>
+    <col min="7" max="7" width="27.1272727272727" customWidth="1"/>
+    <col min="8" max="9" width="9.58181818181818" customWidth="1"/>
+    <col min="10" max="10" width="10.6272727272727" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="21" width="10.7583333333333" customWidth="1"/>
+    <col min="12" max="21" width="10.7545454545455" customWidth="1"/>
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2335,7 +2343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2400,7 +2408,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2459,7 +2467,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2494,7 +2502,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2554,7 +2562,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -2616,7 +2624,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2703,7 +2711,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2765,7 +2773,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2807,7 +2815,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2849,7 +2857,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2873,7 +2881,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2935,7 +2943,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2959,7 +2967,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3015,7 +3023,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3077,7 +3085,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3139,7 +3147,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3171,7 +3179,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3233,7 +3241,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3265,7 +3273,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3327,7 +3335,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3369,7 +3377,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3401,7 +3409,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3463,7 +3471,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3505,7 +3513,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3543,7 +3551,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>118</v>
       </c>
@@ -3587,7 +3595,7 @@
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
@@ -3641,7 +3649,7 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:18">
+    <row r="29" customFormat="1" ht="15" spans="1:18">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -3683,7 +3691,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>131</v>
       </c>
@@ -3737,7 +3745,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
@@ -3799,7 +3807,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15" spans="1:20">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3861,7 +3869,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3889,7 +3897,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
@@ -3945,7 +3953,7 @@
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15" spans="1:20">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -4049,7 +4057,7 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15.75" spans="1:20">
+    <row r="37" customFormat="1" ht="15" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -4091,7 +4099,7 @@
         <v>45712</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15.75" spans="1:20">
+    <row r="38" customFormat="1" ht="15" spans="1:20">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4120,7 +4128,7 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
     </row>
-    <row r="39" customFormat="1" ht="15.75" spans="1:20">
+    <row r="39" customFormat="1" ht="15" spans="1:20">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -4142,7 +4150,7 @@
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
     </row>
-    <row r="40" customFormat="1" ht="15.75" spans="1:20">
+    <row r="40" customFormat="1" ht="15" spans="1:20">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -4164,7 +4172,7 @@
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
     </row>
-    <row r="41" customFormat="1" ht="15.75" spans="1:20">
+    <row r="41" customFormat="1" ht="15" spans="1:20">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
update tutor records and read DMBOK
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -491,11 +491,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -993,7 +993,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1002,10 +1002,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1014,7 +1014,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1194,10 +1194,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1212,13 +1212,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1541,24 +1541,24 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="5.58181818181818" customWidth="1"/>
-    <col min="3" max="3" width="10.6636363636364" customWidth="1"/>
+    <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
+    <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="30.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="30.4583333333333" customWidth="1"/>
     <col min="6" max="6" width="7.5" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="9.87272727272727" customWidth="1"/>
-    <col min="9" max="9" width="9.12727272727273" customWidth="1"/>
-    <col min="10" max="10" width="10.8363636363636" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="9.125" customWidth="1"/>
+    <col min="10" max="10" width="10.8333333333333" customWidth="1"/>
     <col min="11" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:20">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15" spans="1:20">
+    <row r="2" customFormat="1" ht="15.75" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15" spans="1:20">
+    <row r="3" customFormat="1" ht="15.75" spans="1:20">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1724,7 +1724,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15" spans="1:20">
+    <row r="4" customFormat="1" ht="15.75" spans="1:20">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1741,26 +1741,26 @@
       <c r="L4" s="21">
         <v>45717</v>
       </c>
-      <c r="M4" s="22">
+      <c r="M4" s="21">
         <v>45724</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="21">
         <v>45731</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="21">
         <v>45738</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="21">
         <v>45752</v>
       </c>
-      <c r="Q4" s="22">
+      <c r="Q4" s="21">
         <v>45759</v>
       </c>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
       <c r="T4" s="22"/>
     </row>
-    <row r="5" customFormat="1" ht="15" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="6" customFormat="1" ht="15" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1852,7 +1852,7 @@
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
     </row>
-    <row r="7" customFormat="1" ht="15" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15" spans="1:20">
+    <row r="8" customFormat="1" ht="15.75" spans="1:20">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1956,7 +1956,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="9" customFormat="1" ht="15" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1982,7 +1982,7 @@
       <c r="S9" s="22"/>
       <c r="T9" s="22"/>
     </row>
-    <row r="10" customFormat="1" ht="15" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2086,7 +2086,7 @@
         <v>45718</v>
       </c>
     </row>
-    <row r="12" ht="15" spans="1:13">
+    <row r="12" ht="15.75" spans="1:13">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2107,12 +2107,12 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="19" s="20" customFormat="1" ht="15"/>
-    <row r="20" s="20" customFormat="1" ht="15"/>
-    <row r="21" s="20" customFormat="1" ht="15"/>
-    <row r="22" s="20" customFormat="1" ht="15"/>
-    <row r="23" s="20" customFormat="1" ht="15"/>
-    <row r="24" s="20" customFormat="1" ht="15" spans="1:9">
+    <row r="19" s="20" customFormat="1" ht="15.75"/>
+    <row r="20" s="20" customFormat="1" ht="15.75"/>
+    <row r="21" s="20" customFormat="1" ht="15.75"/>
+    <row r="22" s="20" customFormat="1" ht="15.75"/>
+    <row r="23" s="20" customFormat="1" ht="15.75"/>
+    <row r="24" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A24" s="26"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -2123,7 +2123,7 @@
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" s="20" customFormat="1" ht="15" spans="1:9">
+    <row r="25" s="20" customFormat="1" ht="15.75" spans="1:9">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -2134,7 +2134,7 @@
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" ht="17.5" spans="2:13">
+    <row r="26" ht="18.75" spans="2:13">
       <c r="B26" s="8" t="s">
         <v>49</v>
       </c>
@@ -2150,7 +2150,7 @@
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
     </row>
-    <row r="27" ht="17.5" spans="2:13">
+    <row r="27" ht="18.75" spans="2:13">
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -2164,7 +2164,7 @@
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
     </row>
-    <row r="28" ht="17.5" spans="2:12">
+    <row r="28" ht="18.75" spans="2:12">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2176,7 +2176,7 @@
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
     </row>
-    <row r="29" ht="17.5" spans="2:13">
+    <row r="29" ht="18.75" spans="2:13">
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -2190,7 +2190,7 @@
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
     </row>
-    <row r="30" ht="17.5" spans="2:13">
+    <row r="30" ht="18.75" spans="2:13">
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2263,22 +2263,22 @@
       <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="4.58181818181818" customWidth="1"/>
-    <col min="3" max="3" width="10.8727272727273" customWidth="1"/>
+    <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="18.5818181818182" customWidth="1"/>
-    <col min="6" max="6" width="7.33636363636364" customWidth="1"/>
-    <col min="7" max="7" width="27.1272727272727" customWidth="1"/>
-    <col min="8" max="9" width="9.58181818181818" customWidth="1"/>
-    <col min="10" max="10" width="10.6272727272727" customWidth="1"/>
+    <col min="5" max="5" width="18.5833333333333" customWidth="1"/>
+    <col min="6" max="6" width="7.33333333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.125" customWidth="1"/>
+    <col min="8" max="9" width="9.58333333333333" customWidth="1"/>
+    <col min="10" max="10" width="10.625" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="21" width="10.7545454545455" customWidth="1"/>
+    <col min="12" max="21" width="10.7583333333333" customWidth="1"/>
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" spans="1:21">
+    <row r="1" ht="15.75" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15" spans="1:21">
+    <row r="2" customFormat="1" ht="15.75" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15" spans="1:19">
+    <row r="3" customFormat="1" ht="15.75" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15" spans="1:11">
+    <row r="4" customFormat="1" ht="15.75" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15" spans="1:20">
+    <row r="5" customFormat="1" ht="15.75" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15" spans="1:20">
+    <row r="6" customFormat="1" ht="15.75" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15" spans="1:20">
+    <row r="7" customFormat="1" ht="15.75" spans="1:20">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -2711,7 +2711,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="1" ht="15" spans="1:20">
+    <row r="9" customFormat="1" ht="15.75" spans="1:20">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15" spans="1:20">
+    <row r="10" customFormat="1" ht="15.75" spans="1:20">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2815,7 +2815,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15" spans="1:20">
+    <row r="11" customFormat="1" ht="15.75" spans="1:20">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2857,7 +2857,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15" spans="1:20">
+    <row r="12" customFormat="1" ht="15.75" spans="1:20">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2881,7 +2881,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" customFormat="1" ht="15" spans="1:20">
+    <row r="13" customFormat="1" ht="15.75" spans="1:20">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15" spans="1:20">
+    <row r="14" customFormat="1" ht="15.75" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2967,7 +2967,7 @@
       <c r="S14" s="16"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" customFormat="1" ht="15" spans="1:20">
+    <row r="15" customFormat="1" ht="15.75" spans="1:20">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" customFormat="1" ht="15" spans="1:20">
+    <row r="16" customFormat="1" ht="15.75" spans="1:20">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15" spans="1:20">
+    <row r="17" customFormat="1" ht="15.75" spans="1:20">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15" spans="1:20">
+    <row r="18" customFormat="1" ht="15.75" spans="1:20">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -3179,7 +3179,7 @@
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
     </row>
-    <row r="19" customFormat="1" ht="15" spans="1:20">
+    <row r="19" customFormat="1" ht="15.75" spans="1:20">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15" spans="1:20">
+    <row r="20" customFormat="1" ht="15.75" spans="1:20">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -3273,7 +3273,7 @@
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
     </row>
-    <row r="21" customFormat="1" ht="15" spans="1:20">
+    <row r="21" customFormat="1" ht="15.75" spans="1:20">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15" spans="1:20">
+    <row r="22" customFormat="1" ht="15.75" spans="1:20">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -3377,7 +3377,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15" spans="1:20">
+    <row r="23" customFormat="1" ht="15.75" spans="1:20">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -3409,7 +3409,7 @@
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" customFormat="1" ht="15" spans="1:20">
+    <row r="24" customFormat="1" ht="15.75" spans="1:20">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15" spans="1:20">
+    <row r="25" customFormat="1" ht="15.75" spans="1:20">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -3513,7 +3513,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3551,7 +3551,7 @@
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" customFormat="1" ht="15" spans="1:20">
+    <row r="27" customFormat="1" ht="15.75" spans="1:20">
       <c r="A27" s="5" t="s">
         <v>118</v>
       </c>
@@ -3595,7 +3595,7 @@
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
     </row>
-    <row r="28" customFormat="1" ht="15" spans="1:20">
+    <row r="28" customFormat="1" ht="15.75" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>20</v>
       </c>
@@ -3649,7 +3649,7 @@
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" customFormat="1" ht="15" spans="1:18">
+    <row r="29" customFormat="1" ht="15.75" spans="1:18">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -3691,7 +3691,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" customFormat="1" ht="15" spans="1:20">
+    <row r="30" customFormat="1" ht="15.75" spans="1:20">
       <c r="A30" s="5" t="s">
         <v>131</v>
       </c>
@@ -3745,7 +3745,7 @@
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
     </row>
-    <row r="31" customFormat="1" ht="15" spans="1:20">
+    <row r="31" customFormat="1" ht="15.75" spans="1:20">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15" spans="1:20">
+    <row r="32" customFormat="1" ht="15.75" spans="1:20">
       <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15" spans="1:20">
+    <row r="33" customFormat="1" ht="15.75" spans="1:20">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3897,7 +3897,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15" spans="1:20">
+    <row r="34" customFormat="1" ht="15.75" spans="1:20">
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
     </row>
-    <row r="35" customFormat="1" ht="15" spans="1:20">
+    <row r="35" customFormat="1" ht="15.75" spans="1:20">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="36" customFormat="1" ht="15" spans="1:20">
+    <row r="36" customFormat="1" ht="15.75" spans="1:20">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -4057,7 +4057,7 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15" spans="1:20">
+    <row r="37" customFormat="1" ht="15.75" spans="1:20">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -4099,7 +4099,7 @@
         <v>45712</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15" spans="1:20">
+    <row r="38" customFormat="1" ht="15.75" spans="1:20">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -4128,7 +4128,7 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
     </row>
-    <row r="39" customFormat="1" ht="15" spans="1:20">
+    <row r="39" customFormat="1" ht="15.75" spans="1:20">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -4150,7 +4150,7 @@
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
     </row>
-    <row r="40" customFormat="1" ht="15" spans="1:20">
+    <row r="40" customFormat="1" ht="15.75" spans="1:20">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -4172,7 +4172,7 @@
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
     </row>
-    <row r="41" customFormat="1" ht="15" spans="1:20">
+    <row r="41" customFormat="1" ht="15.75" spans="1:20">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>

</xml_diff>

<commit_message>
study 2.3.6-2.3.8 of csapp and update tutor record
</commit_message>
<xml_diff>
--- a/Sideline/家教带课记录.xlsx
+++ b/Sideline/家教带课记录.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="25600" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Doing" sheetId="1" r:id="rId1"/>
@@ -1189,7 +1189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1266,6 +1266,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1592,24 +1595,24 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="5.58333333333333" customWidth="1"/>
-    <col min="3" max="3" width="11.1833333333333" customWidth="1"/>
+    <col min="1" max="2" width="5.58181818181818" customWidth="1"/>
+    <col min="3" max="3" width="11.1818181818182" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.8166666666667" customWidth="1"/>
+    <col min="5" max="5" width="20.8181818181818" customWidth="1"/>
     <col min="6" max="6" width="7.5" customWidth="1"/>
-    <col min="7" max="7" width="26.5416666666667" customWidth="1"/>
-    <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="9" width="9.125" customWidth="1"/>
-    <col min="10" max="10" width="10.8333333333333" customWidth="1"/>
+    <col min="7" max="7" width="26.5454545454545" customWidth="1"/>
+    <col min="8" max="8" width="9.87272727272727" customWidth="1"/>
+    <col min="9" max="9" width="9.12727272727273" customWidth="1"/>
+    <col min="10" max="10" width="10.8363636363636" customWidth="1"/>
     <col min="11" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:20">
+    <row r="1" ht="15" spans="1:20">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:15">
+    <row r="2" customFormat="1" ht="15" spans="1:16">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1717,13 +1720,16 @@
       <c r="O2" s="21">
         <v>46032</v>
       </c>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="15.75"/>
-    <row r="12" s="2" customFormat="1" ht="15.75"/>
-    <row r="13" s="2" customFormat="1" ht="15.75"/>
-    <row r="14" s="2" customFormat="1" ht="15.75"/>
-    <row r="15" s="2" customFormat="1" ht="15.75"/>
-    <row r="16" s="2" customFormat="1" ht="15.75" spans="1:9">
+      <c r="P2" s="29">
+        <v>46039</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="15"/>
+    <row r="12" s="2" customFormat="1" ht="15"/>
+    <row r="13" s="2" customFormat="1" ht="15"/>
+    <row r="14" s="2" customFormat="1" ht="15"/>
+    <row r="15" s="2" customFormat="1" ht="15"/>
+    <row r="16" s="2" customFormat="1" ht="15" spans="1:9">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -1734,7 +1740,7 @@
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" s="2" customFormat="1" ht="15.75" spans="1:9">
+    <row r="17" s="2" customFormat="1" ht="15" spans="1:9">
       <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -1745,7 +1751,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" ht="18.75" spans="2:13">
+    <row r="18" ht="17.5" spans="2:13">
       <c r="B18" s="9" t="s">
         <v>30</v>
       </c>
@@ -1756,12 +1762,12 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-    </row>
-    <row r="19" ht="18.75" spans="2:13">
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" ht="17.5" spans="2:13">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1770,12 +1776,12 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-    </row>
-    <row r="20" ht="18.75" spans="2:12">
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+    </row>
+    <row r="20" ht="17.5" spans="2:12">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1784,10 +1790,10 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-    </row>
-    <row r="21" ht="18.75" spans="2:13">
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" ht="17.5" spans="2:13">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1796,12 +1802,12 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-    </row>
-    <row r="22" ht="18.75" spans="2:13">
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+    </row>
+    <row r="22" ht="17.5" spans="2:13">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1810,10 +1816,10 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1834,22 +1840,22 @@
       <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="4.58333333333333" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="17.725" customWidth="1"/>
-    <col min="5" max="5" width="23.1833333333333" customWidth="1"/>
-    <col min="6" max="6" width="7.33333333333333" customWidth="1"/>
-    <col min="7" max="7" width="27.125" customWidth="1"/>
-    <col min="8" max="9" width="9.58333333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.625" customWidth="1"/>
-    <col min="11" max="20" width="11.275" customWidth="1"/>
-    <col min="21" max="21" width="10.7583333333333" customWidth="1"/>
+    <col min="1" max="2" width="4.58181818181818" customWidth="1"/>
+    <col min="3" max="3" width="10.8727272727273" customWidth="1"/>
+    <col min="4" max="4" width="17.7272727272727" customWidth="1"/>
+    <col min="5" max="5" width="23.1818181818182" customWidth="1"/>
+    <col min="6" max="6" width="7.33636363636364" customWidth="1"/>
+    <col min="7" max="7" width="27.1272727272727" customWidth="1"/>
+    <col min="8" max="9" width="9.58181818181818" customWidth="1"/>
+    <col min="10" max="10" width="10.6272727272727" customWidth="1"/>
+    <col min="11" max="20" width="11.2727272727273" customWidth="1"/>
+    <col min="21" max="21" width="10.7545454545455" customWidth="1"/>
     <col min="22" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:21">
+    <row r="1" ht="15" spans="1:21">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="15.75" spans="1:21">
+    <row r="2" customFormat="1" ht="15" spans="1:21">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>45248</v>
       </c>
     </row>
-    <row r="3" customFormat="1" ht="15.75" spans="1:19">
+    <row r="3" customFormat="1" ht="15" spans="1:19">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
@@ -2038,7 +2044,7 @@
         <v>45304</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="1:11">
+    <row r="4" customFormat="1" ht="15" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>45294</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="1:20">
+    <row r="5" customFormat="1" ht="15" spans="1:20">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -2133,7 +2139,7 @@
       </c>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" customFormat="1" ht="15.75" spans="1:20">
+    <row r="6" customFormat="1" ht="15" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>39</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>45344</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="15.75" spans="1:20">
+    <row r="7" customFormat="1" ht="15" spans="1:20">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2282,7 +2288,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" customFormat="1" ht="15.75" spans="1:20">
+    <row r="9" customFormat="1" ht="15" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>45263</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="1:20">
+    <row r="10" customFormat="1" ht="15" spans="1:20">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2386,7 +2392,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="11" customFormat="1" ht="15.75" spans="1:20">
+    <row r="11" customFormat="1" ht="15" spans="1:20">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2428,7 +2434,7 @@
         <v>45445</v>
       </c>
     </row>
-    <row r="12" customFormat="1" ht="15.75" spans="1:20">
+    <row r="12" customFormat="1" ht="15" spans="1:20">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2452,7 +2458,7 @@
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="1:20">
+    <row r="13" customFormat="1" ht="15" spans="1:20">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>45453</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="15.75" spans="1:20">
+    <row r="14" customFormat="1" ht="15" spans="1:20">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2538,7 +2544,7 @@
       <c r="S14" s="17"/>
       <c r="T14" s="19"/>
     </row>
-    <row r="15" customFormat="1" ht="15.75" spans="1:20">
+    <row r="15" customFormat="1" ht="15" spans="1:20">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -2594,7 +2600,7 @@
       <c r="S15" s="17"/>
       <c r="T15" s="19"/>
     </row>
-    <row r="16" customFormat="1" ht="15.75" spans="1:20">
+    <row r="16" customFormat="1" ht="15" spans="1:20">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -2656,7 +2662,7 @@
         <v>45461</v>
       </c>
     </row>
-    <row r="17" customFormat="1" ht="15.75" spans="1:20">
+    <row r="17" customFormat="1" ht="15" spans="1:20">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -2718,7 +2724,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="18" customFormat="1" ht="15.75" spans="1:20">
+    <row r="18" customFormat="1" ht="15" spans="1:20">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2750,7 +2756,7 @@
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" customFormat="1" ht="15.75" spans="1:20">
+    <row r="19" customFormat="1" ht="15" spans="1:20">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>45451</v>
       </c>
     </row>
-    <row r="20" customFormat="1" ht="15.75" spans="1:20">
+    <row r="20" customFormat="1" ht="15" spans="1:20">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2844,7 +2850,7 @@
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" customFormat="1" ht="15.75" spans="1:20">
+    <row r="21" customFormat="1" ht="15" spans="1:20">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="22" customFormat="1" ht="15.75" spans="1:20">
+    <row r="22" customFormat="1" ht="15" spans="1:20">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2948,7 +2954,7 @@
         <v>45423</v>
       </c>
     </row>
-    <row r="23" customFormat="1" ht="15.75" spans="1:20">
+    <row r="23" customFormat="1" ht="15" spans="1:20">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2980,7 +2986,7 @@
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
     </row>
-    <row r="24" customFormat="1" ht="15.75" spans="1:20">
+    <row r="24" customFormat="1" ht="15" spans="1:20">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>45325</v>
       </c>
     </row>
-    <row r="25" customFormat="1" ht="15.75" spans="1:20">
+    <row r="25" customFormat="1" ht="15" spans="1:20">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3084,7 +3090,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:20">
+    <row r="26" s="1" customFormat="1" ht="15" spans="1:20">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3122,7 +3128,7 @@
       <c r="S26" s="17"/>
       <c r="T26" s="17"/>
     </row>
-    <row r="27" customFormat="1" ht="15.75" spans="1:20">
+    <row r="27" customFormat="1" ht="15" spans="1:20">
       <c r="A27" s="6" t="s">
         <v>103</v>
       </c>
@@ -3166,7 +3172,7 @@
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
     </row>
-    <row r="28" customFormat="1" ht="15.75" spans="1:20">
+    <row r="28" customFormat="1" ht="15" spans="1:20">
       <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
@@ -3220,7 +3226,7 @@
       <c r="S28" s="17"/>
       <c r="T28" s="17"/>
     </row>
-    <row r="29" customFormat="1" ht="15.75" spans="1:18">
+    <row r="29" customFormat="1" ht="15" spans="1:18">
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
@@ -3262,7 +3268,7 @@
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
     </row>
-    <row r="30" customFormat="1" ht="15.75" spans="1:20">
+    <row r="30" customFormat="1" ht="15" spans="1:20">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -3316,7 +3322,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" customFormat="1" ht="15.75" spans="1:20">
+    <row r="31" customFormat="1" ht="15" spans="1:20">
       <c r="A31" s="6" t="s">
         <v>20</v>
       </c>
@@ -3378,7 +3384,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="32" customFormat="1" ht="15.75" spans="1:20">
+    <row r="32" customFormat="1" ht="15" spans="1:20">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>45627</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="1:20">
+    <row r="33" customFormat="1" ht="15" spans="1:20">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -3468,7 +3474,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" customFormat="1" ht="15.75" spans="1:20">
+    <row r="34" customFormat="1" ht="15" spans="1:20">
       <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
@@ -3524,7 +3530,7 @@
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
     </row>
-    <row r="35" customFormat="1" ht="15.75" spans="1:20">
+    <row r="35" customFormat="1" ht="15" spans="1:20">
       <c r="A35" s="5" t="s">
         <v>20</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="36" customFormat="1" ht="15.75" spans="1:20">
+    <row r="36" customFormat="1" ht="15" spans="1:20">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3628,7 +3634,7 @@
         <v>45691</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15.75" spans="1:20">
+    <row r="37" customFormat="1" ht="15" spans="1:20">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3670,7 +3676,7 @@
         <v>45712</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15.75" spans="1:20">
+    <row r="38" customFormat="1" ht="15" spans="1:20">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3699,7 +3705,7 @@
       <c r="S38" s="22"/>
       <c r="T38" s="22"/>
     </row>
-    <row r="39" customFormat="1" ht="15.75" spans="1:20">
+    <row r="39" customFormat="1" ht="15" spans="1:20">
       <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
@@ -3761,7 +3767,7 @@
         <v>45592</v>
       </c>
     </row>
-    <row r="40" customFormat="1" ht="15.75" spans="1:20">
+    <row r="40" customFormat="1" ht="15" spans="1:20">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3803,7 +3809,7 @@
         <v>45718</v>
       </c>
     </row>
-    <row r="41" customFormat="1" ht="15.75" spans="1:13">
+    <row r="41" customFormat="1" ht="15" spans="1:13">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -3824,7 +3830,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="42" customFormat="1" ht="15.75" spans="1:20">
+    <row r="42" customFormat="1" ht="15" spans="1:20">
       <c r="A42" s="5" t="s">
         <v>20</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>45623</v>
       </c>
     </row>
-    <row r="43" customFormat="1" ht="15.75" spans="1:20">
+    <row r="43" customFormat="1" ht="15" spans="1:20">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -3928,7 +3934,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="44" customFormat="1" ht="15.75" spans="1:20">
+    <row r="44" customFormat="1" ht="15" spans="1:20">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -4006,7 +4012,7 @@
       <c r="S45" s="22"/>
       <c r="T45" s="22"/>
     </row>
-    <row r="46" customFormat="1" ht="15.75" spans="1:20">
+    <row r="46" customFormat="1" ht="15" spans="1:20">
       <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="47" customFormat="1" ht="15.75" spans="1:20">
+    <row r="47" customFormat="1" ht="15" spans="1:20">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -4110,7 +4116,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="48" customFormat="1" ht="15.75" spans="1:20">
+    <row r="48" customFormat="1" ht="15" spans="1:20">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -4142,7 +4148,7 @@
       <c r="S48" s="22"/>
       <c r="T48" s="22"/>
     </row>
-    <row r="49" s="2" customFormat="1" ht="15.75" spans="1:16">
+    <row r="49" s="2" customFormat="1" ht="15" spans="1:16">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
@@ -4192,7 +4198,7 @@
         <v>45823</v>
       </c>
     </row>
-    <row r="50" customFormat="1" ht="15.75" spans="1:20">
+    <row r="50" customFormat="1" ht="15" spans="1:20">
       <c r="A50" s="5" t="s">
         <v>20</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>45746</v>
       </c>
     </row>
-    <row r="51" customFormat="1" ht="15.75" spans="1:20">
+    <row r="51" customFormat="1" ht="15" spans="1:20">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -4296,7 +4302,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="52" customFormat="1" ht="15.75" spans="1:20">
+    <row r="52" customFormat="1" ht="15" spans="1:20">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -4338,7 +4344,7 @@
         <v>45822</v>
       </c>
     </row>
-    <row r="53" customFormat="1" ht="15.75" spans="1:12">
+    <row r="53" customFormat="1" ht="15" spans="1:12">
       <c r="A53" s="5" t="s">
         <v>20</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="54" customFormat="1" ht="15.75" spans="1:20">
+    <row r="54" customFormat="1" ht="15" spans="1:20">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -4398,7 +4404,7 @@
       <c r="S54" s="22"/>
       <c r="T54" s="22"/>
     </row>
-    <row r="55" customFormat="1" ht="15.75" spans="1:20">
+    <row r="55" customFormat="1" ht="15" spans="1:20">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -4420,7 +4426,7 @@
       <c r="S55" s="22"/>
       <c r="T55" s="22"/>
     </row>
-    <row r="56" customFormat="1" ht="15.75" spans="1:20">
+    <row r="56" customFormat="1" ht="15" spans="1:20">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -4442,7 +4448,7 @@
       <c r="S56" s="22"/>
       <c r="T56" s="22"/>
     </row>
-    <row r="57" customFormat="1" ht="15.75" spans="1:20">
+    <row r="57" customFormat="1" ht="15" spans="1:20">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -4464,7 +4470,7 @@
       <c r="S57" s="22"/>
       <c r="T57" s="22"/>
     </row>
-    <row r="58" customFormat="1" ht="15.75" spans="1:20">
+    <row r="58" customFormat="1" ht="15" spans="1:20">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -4486,7 +4492,7 @@
       <c r="S58" s="27"/>
       <c r="T58" s="27"/>
     </row>
-    <row r="59" customFormat="1" ht="15.75" spans="1:20">
+    <row r="59" customFormat="1" ht="15" spans="1:20">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -4508,7 +4514,7 @@
       <c r="S59" s="27"/>
       <c r="T59" s="27"/>
     </row>
-    <row r="60" customFormat="1" ht="15.75" spans="1:20">
+    <row r="60" customFormat="1" ht="15" spans="1:20">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>

</xml_diff>